<commit_message>
nutrient tweaks based on pH values
</commit_message>
<xml_diff>
--- a/meta_data/hoaglands_recipes_p_v1.xlsx
+++ b/meta_data/hoaglands_recipes_p_v1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monik\Documents\git\2025_g34p\meta_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF6D801-5CAC-4D9B-9588-35615AFBE854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52D2AF4-DC53-4CBE-9896-87A9D0A98FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CEBD6CB8-EBC1-4974-8449-BAC066E52B02}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{672A70A4-BEEB-4E9F-898A-72ED4A72F9C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="recipes" sheetId="4" r:id="rId1"/>
-    <sheet name="print" sheetId="5" r:id="rId2"/>
+    <sheet name="recipes_v1" sheetId="4" r:id="rId1"/>
+    <sheet name="recipes_v2" sheetId="6" r:id="rId2"/>
+    <sheet name="print" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="105">
   <si>
     <t>Primary N addition compounds</t>
   </si>
@@ -1449,6 +1450,15 @@
   </si>
   <si>
     <t>mL per 20 L</t>
+  </si>
+  <si>
+    <t>BASE</t>
+  </si>
+  <si>
+    <t>diff. base</t>
+  </si>
+  <si>
+    <t>mL for 0.5 L</t>
   </si>
 </sst>
 </file>
@@ -1458,7 +1468,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1571,8 +1581,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1652,6 +1676,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2148,7 +2178,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2334,17 +2364,53 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2771,8 +2837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C991C1-A1AF-4EC8-80EB-A4FE0F14FB5F}">
   <dimension ref="B1:AB44"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5428,12 +5494,3123 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1110D87-9739-4E9A-9895-32B9F5C305B9}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:AF53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15" style="2" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" customWidth="1"/>
+    <col min="9" max="9" width="15" style="2" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" customWidth="1"/>
+    <col min="16" max="16" width="15" style="2" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" customWidth="1"/>
+    <col min="23" max="23" width="15" style="2" customWidth="1"/>
+    <col min="25" max="25" width="13" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="49" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="47.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="113"/>
+    </row>
+    <row r="2" spans="2:32" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="108" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="161"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="162"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="162"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="162"/>
+      <c r="AD2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="9"/>
+    </row>
+    <row r="3" spans="2:32" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="28">
+        <f>C40/AE35</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="28">
+        <f>J40/AE35</f>
+        <v>0.49999515722864341</v>
+      </c>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="162"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="28">
+        <f>Q40/AE35</f>
+        <v>0.99999031445728681</v>
+      </c>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="30"/>
+      <c r="U3" s="162"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="X3" s="28">
+        <f>X40/AE35</f>
+        <v>1.9999806289145736</v>
+      </c>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="162"/>
+      <c r="AD3" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE3" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF3" s="69" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:32" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B4" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="58"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="58"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="163"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="58"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="163"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="X4" s="58"/>
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="45"/>
+      <c r="AA4" s="56"/>
+      <c r="AB4" s="163"/>
+      <c r="AD4" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE4" s="17">
+        <v>115.03</v>
+      </c>
+      <c r="AF4" s="18">
+        <v>115.03</v>
+      </c>
+    </row>
+    <row r="5" spans="2:32" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="163" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="163" t="s">
+        <v>104</v>
+      </c>
+      <c r="P5" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="T5" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" s="163" t="s">
+        <v>104</v>
+      </c>
+      <c r="W5" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y5" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z5" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB5" s="163" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD5" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE5" s="17">
+        <v>101.11</v>
+      </c>
+      <c r="AF5" s="18">
+        <f>AE5*2</f>
+        <v>202.22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B6" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="53">
+        <v>1</v>
+      </c>
+      <c r="D6" s="53">
+        <v>115.3</v>
+      </c>
+      <c r="E6" s="149">
+        <v>0</v>
+      </c>
+      <c r="F6" s="151">
+        <f t="shared" ref="F6:F8" si="0">IF(OR(D6=0,E6=0),0,(D6*1000)/(1000/(C6*E6)))</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="164">
+        <f>E6/2</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="53">
+        <v>1</v>
+      </c>
+      <c r="K6" s="53">
+        <v>115.3</v>
+      </c>
+      <c r="L6" s="157">
+        <v>0.5</v>
+      </c>
+      <c r="M6" s="55">
+        <f t="shared" ref="M6:M8" si="1">IF(OR(K6=0,L6=0),0,(K6*1000)/(1000/(J6*L6)))</f>
+        <v>57.65</v>
+      </c>
+      <c r="N6" s="165">
+        <f>L6/2</f>
+        <v>0.25</v>
+      </c>
+      <c r="P6" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q6" s="53">
+        <v>1</v>
+      </c>
+      <c r="R6" s="53">
+        <v>115.3</v>
+      </c>
+      <c r="S6" s="53">
+        <v>1</v>
+      </c>
+      <c r="T6" s="55">
+        <f t="shared" ref="T6:T8" si="2">IF(OR(R6=0,S6=0),0,(R6*1000)/(1000/(Q6*S6)))</f>
+        <v>115.3</v>
+      </c>
+      <c r="U6" s="165">
+        <f>S6/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="W6" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="X6" s="53">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="53">
+        <v>115.3</v>
+      </c>
+      <c r="Z6" s="53">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="55">
+        <f t="shared" ref="AA6:AA8" si="3">IF(OR(Y6=0,Z6=0),0,(Y6*1000)/(1000/(X6*Z6)))</f>
+        <v>230.6</v>
+      </c>
+      <c r="AB6" s="165">
+        <f>Z6/2</f>
+        <v>1</v>
+      </c>
+      <c r="AD6" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE6" s="17">
+        <v>236.15</v>
+      </c>
+      <c r="AF6" s="18">
+        <f>AE6*2</f>
+        <v>472.3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B7" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="24">
+        <v>2</v>
+      </c>
+      <c r="D7" s="24">
+        <v>101.1</v>
+      </c>
+      <c r="E7" s="160">
+        <v>2</v>
+      </c>
+      <c r="F7" s="153">
+        <f t="shared" si="0"/>
+        <v>404.4</v>
+      </c>
+      <c r="G7" s="164">
+        <f t="shared" ref="G7:G18" si="4">E7/2</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="24">
+        <v>2</v>
+      </c>
+      <c r="K7" s="24">
+        <v>101.1</v>
+      </c>
+      <c r="L7" s="156">
+        <v>2</v>
+      </c>
+      <c r="M7" s="32">
+        <f t="shared" si="1"/>
+        <v>404.4</v>
+      </c>
+      <c r="N7" s="165">
+        <f t="shared" ref="N7:N18" si="5">L7/2</f>
+        <v>1</v>
+      </c>
+      <c r="P7" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q7" s="24">
+        <v>2</v>
+      </c>
+      <c r="R7" s="24">
+        <v>101.1</v>
+      </c>
+      <c r="S7" s="24">
+        <v>2</v>
+      </c>
+      <c r="T7" s="32">
+        <f t="shared" si="2"/>
+        <v>404.4</v>
+      </c>
+      <c r="U7" s="165">
+        <f t="shared" ref="U7:U9" si="6">S7/2</f>
+        <v>1</v>
+      </c>
+      <c r="W7" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="X7" s="24">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="24">
+        <v>101.1</v>
+      </c>
+      <c r="Z7" s="24">
+        <v>2</v>
+      </c>
+      <c r="AA7" s="32">
+        <f t="shared" si="3"/>
+        <v>404.4</v>
+      </c>
+      <c r="AB7" s="165">
+        <f t="shared" ref="AB7:AB9" si="7">Z7/2</f>
+        <v>1</v>
+      </c>
+      <c r="AD7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE7" s="17">
+        <v>80.040000000000006</v>
+      </c>
+      <c r="AF7" s="18">
+        <v>80.040000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B8" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="112">
+        <v>2</v>
+      </c>
+      <c r="D8" s="24">
+        <v>164.08799999999999</v>
+      </c>
+      <c r="E8" s="160">
+        <v>1.5</v>
+      </c>
+      <c r="F8" s="153">
+        <f t="shared" si="0"/>
+        <v>492.26400000000001</v>
+      </c>
+      <c r="G8" s="164">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="I8" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="24">
+        <v>2</v>
+      </c>
+      <c r="K8" s="24">
+        <v>164.08799999999999</v>
+      </c>
+      <c r="L8" s="156">
+        <v>1.5</v>
+      </c>
+      <c r="M8" s="32">
+        <f t="shared" si="1"/>
+        <v>492.26400000000001</v>
+      </c>
+      <c r="N8" s="165">
+        <f t="shared" si="5"/>
+        <v>0.75</v>
+      </c>
+      <c r="P8" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q8" s="24">
+        <v>2</v>
+      </c>
+      <c r="R8" s="24">
+        <v>164.08799999999999</v>
+      </c>
+      <c r="S8" s="156">
+        <v>1.25</v>
+      </c>
+      <c r="T8" s="32">
+        <f t="shared" si="2"/>
+        <v>410.22</v>
+      </c>
+      <c r="U8" s="165">
+        <f t="shared" si="6"/>
+        <v>0.625</v>
+      </c>
+      <c r="W8" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="X8" s="24">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="24">
+        <v>164.08799999999999</v>
+      </c>
+      <c r="Z8" s="156">
+        <v>1.5</v>
+      </c>
+      <c r="AA8" s="32">
+        <f t="shared" si="3"/>
+        <v>492.26400000000001</v>
+      </c>
+      <c r="AB8" s="165">
+        <f t="shared" si="7"/>
+        <v>0.75</v>
+      </c>
+      <c r="AD8" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE8" s="17">
+        <v>80.040000000000006</v>
+      </c>
+      <c r="AF8" s="18">
+        <f>AE8*8</f>
+        <v>640.32000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B9" s="111" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="24">
+        <v>1</v>
+      </c>
+      <c r="D9" s="114">
+        <v>80.043000000000006</v>
+      </c>
+      <c r="E9" s="160">
+        <v>2.5</v>
+      </c>
+      <c r="F9" s="153">
+        <f>IF(OR(D9=0,E9=0),0,(D9*1000)/(1000/(C9*E9)))</f>
+        <v>200.10749999999999</v>
+      </c>
+      <c r="G9" s="164">
+        <f t="shared" si="4"/>
+        <v>1.25</v>
+      </c>
+      <c r="I9" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="24">
+        <v>1</v>
+      </c>
+      <c r="K9" s="24">
+        <v>80.043000000000006</v>
+      </c>
+      <c r="L9" s="156">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M9" s="32">
+        <f>IF(OR(K9=0,L9=0),0,(K9*1000)/(1000/(J9*L9)))</f>
+        <v>184.09889999999999</v>
+      </c>
+      <c r="N9" s="165">
+        <f t="shared" si="5"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="P9" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q9" s="24">
+        <v>1</v>
+      </c>
+      <c r="R9" s="24">
+        <v>80.043000000000006</v>
+      </c>
+      <c r="S9" s="156">
+        <v>2.5</v>
+      </c>
+      <c r="T9" s="32">
+        <f>IF(OR(R9=0,S9=0),0,(R9*1000)/(1000/(Q9*S9)))</f>
+        <v>200.10749999999999</v>
+      </c>
+      <c r="U9" s="165">
+        <f t="shared" si="6"/>
+        <v>1.25</v>
+      </c>
+      <c r="W9" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="X9" s="24">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="24">
+        <v>80.043000000000006</v>
+      </c>
+      <c r="Z9" s="156">
+        <v>1.5</v>
+      </c>
+      <c r="AA9" s="32">
+        <f>IF(OR(Y9=0,Z9=0),0,(Y9*1000)/(1000/(X9*Z9)))</f>
+        <v>120.06450000000001</v>
+      </c>
+      <c r="AB9" s="165">
+        <f t="shared" si="7"/>
+        <v>0.75</v>
+      </c>
+      <c r="AD9" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE9" s="17">
+        <v>136.09</v>
+      </c>
+      <c r="AF9" s="18">
+        <v>136.09</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="33"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="164"/>
+      <c r="I10" s="33"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="165"/>
+      <c r="P10" s="33"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="165"/>
+      <c r="W10" s="33"/>
+      <c r="AA10" s="34"/>
+      <c r="AB10" s="165"/>
+      <c r="AD10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE10" s="17">
+        <v>74.55</v>
+      </c>
+      <c r="AF10" s="18">
+        <v>74.55</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B11" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="164"/>
+      <c r="I11" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="165"/>
+      <c r="P11" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="56"/>
+      <c r="U11" s="163"/>
+      <c r="W11" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="X11" s="45"/>
+      <c r="Y11" s="45"/>
+      <c r="Z11" s="45"/>
+      <c r="AA11" s="56"/>
+      <c r="AB11" s="163"/>
+      <c r="AD11" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE11" s="17">
+        <v>100.09</v>
+      </c>
+      <c r="AF11" s="18">
+        <v>100.09</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="163" t="s">
+        <v>104</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="M12" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="163" t="s">
+        <v>104</v>
+      </c>
+      <c r="P12" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="R12" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="S12" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="T12" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" s="163" t="s">
+        <v>104</v>
+      </c>
+      <c r="W12" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="X12" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y12" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z12" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB12" s="163" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD12" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE12" s="17">
+        <v>246.48</v>
+      </c>
+      <c r="AF12" s="18">
+        <f>AE12*2</f>
+        <v>492.96</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="94" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="53">
+        <v>1</v>
+      </c>
+      <c r="D13" s="53">
+        <v>136.08600000000001</v>
+      </c>
+      <c r="E13" s="149">
+        <v>0</v>
+      </c>
+      <c r="F13" s="154">
+        <f>IF(OR(C13=0, E13=0), 0, (D13*1000)/(1000/(C13*E13)))</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="164">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="94" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="53">
+        <v>1</v>
+      </c>
+      <c r="K13" s="53">
+        <v>136.08600000000001</v>
+      </c>
+      <c r="L13" s="157">
+        <v>0</v>
+      </c>
+      <c r="M13" s="54">
+        <f>IF(OR(J13=0, L13=0), 0, (K13*1000)/(1000/(J13*L13)))</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="165">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="94" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q13" s="53">
+        <v>1</v>
+      </c>
+      <c r="R13" s="53">
+        <v>136.08600000000001</v>
+      </c>
+      <c r="S13" s="53">
+        <v>0</v>
+      </c>
+      <c r="T13" s="54">
+        <v>0</v>
+      </c>
+      <c r="U13" s="166">
+        <f>S13/2</f>
+        <v>0</v>
+      </c>
+      <c r="W13" s="94" t="s">
+        <v>68</v>
+      </c>
+      <c r="X13" s="53">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="53">
+        <v>136.08600000000001</v>
+      </c>
+      <c r="Z13" s="53">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="54">
+        <f>IF(OR(X13=0, Z13=0), 0, (Y13*1000)/(1000/(X13*Z13)))</f>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="166">
+        <f>Z13/2</f>
+        <v>0</v>
+      </c>
+      <c r="AD13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE13" s="20">
+        <v>38.5</v>
+      </c>
+      <c r="AF13" s="21">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="96" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="24">
+        <v>1</v>
+      </c>
+      <c r="D14" s="24">
+        <v>74.555000000000007</v>
+      </c>
+      <c r="E14" s="160">
+        <v>0</v>
+      </c>
+      <c r="F14" s="155">
+        <f t="shared" ref="F14:F16" si="8">IF(OR(C14=0, E14=0), 0, (D14*1000)/(1000/(C14*E14)))</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="164">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="96" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="24">
+        <v>1</v>
+      </c>
+      <c r="K14" s="24">
+        <v>74.555000000000007</v>
+      </c>
+      <c r="L14" s="24">
+        <v>0</v>
+      </c>
+      <c r="M14" s="35">
+        <f t="shared" ref="M14:M16" si="9">IF(OR(J14=0, L14=0), 0, (K14*1000)/(1000/(J14*L14)))</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="165">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="96" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="24">
+        <v>1</v>
+      </c>
+      <c r="R14" s="24">
+        <v>74.555000000000007</v>
+      </c>
+      <c r="S14" s="24">
+        <v>0</v>
+      </c>
+      <c r="T14" s="35">
+        <v>0</v>
+      </c>
+      <c r="U14" s="166">
+        <f t="shared" ref="U14:U18" si="10">S14/2</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="96" t="s">
+        <v>6</v>
+      </c>
+      <c r="X14" s="24">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="24">
+        <v>74.555000000000007</v>
+      </c>
+      <c r="Z14" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="35">
+        <f t="shared" ref="AA14:AA16" si="11">IF(OR(X14=0, Z14=0), 0, (Y14*1000)/(1000/(X14*Z14)))</f>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="166">
+        <f t="shared" ref="AB14:AB18" si="12">Z14/2</f>
+        <v>0</v>
+      </c>
+      <c r="AD14" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE14" s="70"/>
+      <c r="AF14" s="71"/>
+    </row>
+    <row r="15" spans="2:32" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B15" s="97" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="24">
+        <v>1</v>
+      </c>
+      <c r="D15" s="24">
+        <v>100.087</v>
+      </c>
+      <c r="E15" s="160">
+        <v>1</v>
+      </c>
+      <c r="F15" s="155">
+        <f t="shared" si="8"/>
+        <v>100.087</v>
+      </c>
+      <c r="G15" s="164">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="97" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="24">
+        <v>1</v>
+      </c>
+      <c r="K15" s="24">
+        <v>100.087</v>
+      </c>
+      <c r="L15" s="156">
+        <v>1</v>
+      </c>
+      <c r="M15" s="35">
+        <f t="shared" si="9"/>
+        <v>100.087</v>
+      </c>
+      <c r="N15" s="165">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="P15" s="97" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q15" s="24">
+        <v>1</v>
+      </c>
+      <c r="R15" s="24">
+        <v>100.087</v>
+      </c>
+      <c r="S15" s="156">
+        <v>1.5</v>
+      </c>
+      <c r="T15" s="35">
+        <v>0</v>
+      </c>
+      <c r="U15" s="166">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="W15" s="97" t="s">
+        <v>71</v>
+      </c>
+      <c r="X15" s="24">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="24">
+        <v>100.087</v>
+      </c>
+      <c r="Z15" s="156">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="35">
+        <f t="shared" si="11"/>
+        <v>100.087</v>
+      </c>
+      <c r="AB15" s="166">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="AD15" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE15" s="22">
+        <v>197.92</v>
+      </c>
+      <c r="AF15" s="18">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B16" s="98" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="24">
+        <v>2</v>
+      </c>
+      <c r="D16" s="24">
+        <v>246.48</v>
+      </c>
+      <c r="E16" s="152">
+        <v>1</v>
+      </c>
+      <c r="F16" s="155">
+        <f t="shared" si="8"/>
+        <v>492.96</v>
+      </c>
+      <c r="G16" s="164">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="I16" s="98" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="24">
+        <v>2</v>
+      </c>
+      <c r="K16" s="24">
+        <v>246.48</v>
+      </c>
+      <c r="L16" s="24">
+        <v>1</v>
+      </c>
+      <c r="M16" s="35">
+        <f t="shared" si="9"/>
+        <v>492.96</v>
+      </c>
+      <c r="N16" s="165">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="P16" s="98" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q16" s="24">
+        <v>2</v>
+      </c>
+      <c r="R16" s="24">
+        <v>246.48</v>
+      </c>
+      <c r="S16" s="24">
+        <v>1</v>
+      </c>
+      <c r="T16" s="35">
+        <f t="shared" ref="T16:T18" si="13">(R16*1000)/(1000/(Q16*S16))</f>
+        <v>492.96</v>
+      </c>
+      <c r="U16" s="166">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="W16" s="98" t="s">
+        <v>73</v>
+      </c>
+      <c r="X16" s="24">
+        <v>2</v>
+      </c>
+      <c r="Y16" s="24">
+        <v>246.48</v>
+      </c>
+      <c r="Z16" s="24">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="35">
+        <f t="shared" si="11"/>
+        <v>492.96</v>
+      </c>
+      <c r="AB16" s="166">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="AD16" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE16" s="22">
+        <v>61.83</v>
+      </c>
+      <c r="AF16" s="18">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B17" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="24">
+        <v>1</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="152">
+        <v>1</v>
+      </c>
+      <c r="F17" s="155"/>
+      <c r="G17" s="164">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="24">
+        <v>1</v>
+      </c>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24">
+        <v>1</v>
+      </c>
+      <c r="M17" s="35"/>
+      <c r="N17" s="165">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="P17" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q17" s="24">
+        <v>1</v>
+      </c>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24">
+        <v>1</v>
+      </c>
+      <c r="T17" s="35">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="U17" s="166">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="W17" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="X17" s="24">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="24">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="35"/>
+      <c r="AB17" s="166">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="AD17" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE17" s="17">
+        <v>287.60000000000002</v>
+      </c>
+      <c r="AF17" s="18">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B18" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="24">
+        <v>1</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24">
+        <v>1</v>
+      </c>
+      <c r="F18" s="35">
+        <f t="shared" ref="F18" si="14">(D18*1000)/(1000/(C18*E18))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="164">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="24">
+        <v>1</v>
+      </c>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24">
+        <v>1</v>
+      </c>
+      <c r="M18" s="35">
+        <f t="shared" ref="M18" si="15">(K18*1000)/(1000/(J18*L18))</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="165">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="P18" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q18" s="24">
+        <v>1</v>
+      </c>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24">
+        <v>1</v>
+      </c>
+      <c r="T18" s="35">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="U18" s="166">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="W18" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="X18" s="24">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="35">
+        <f t="shared" ref="AA18" si="16">(Y18*1000)/(1000/(X18*Z18))</f>
+        <v>0</v>
+      </c>
+      <c r="AB18" s="166">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="AD18" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE18" s="17">
+        <v>249.68</v>
+      </c>
+      <c r="AF18" s="18">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="33"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="165"/>
+      <c r="I19" s="33"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="165"/>
+      <c r="P19" s="33"/>
+      <c r="T19" s="34"/>
+      <c r="U19" s="165"/>
+      <c r="W19" s="33"/>
+      <c r="AA19" s="34"/>
+      <c r="AB19" s="165"/>
+      <c r="AD19" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE19" s="20">
+        <v>161.94999999999999</v>
+      </c>
+      <c r="AF19" s="21">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="163"/>
+      <c r="I20" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="163"/>
+      <c r="P20" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="45"/>
+      <c r="T20" s="56"/>
+      <c r="U20" s="163"/>
+      <c r="W20" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="X20" s="45"/>
+      <c r="Y20" s="45"/>
+      <c r="Z20" s="45"/>
+      <c r="AA20" s="56"/>
+      <c r="AB20" s="163"/>
+      <c r="AD20" s="22"/>
+      <c r="AE20" s="17"/>
+      <c r="AF20" s="22"/>
+    </row>
+    <row r="21" spans="2:32" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="163"/>
+      <c r="I21" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="L21" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" s="163"/>
+      <c r="P21" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="R21" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="S21" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="T21" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="U21" s="163"/>
+      <c r="W21" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="X21" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y21" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z21" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA21" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB21" s="163"/>
+      <c r="AD21" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE21" s="77"/>
+      <c r="AF21" s="78"/>
+    </row>
+    <row r="22" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="53">
+        <f>C6</f>
+        <v>1</v>
+      </c>
+      <c r="D22" s="53">
+        <v>14.006</v>
+      </c>
+      <c r="E22" s="53">
+        <f>E6</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="54">
+        <f t="shared" ref="F22:F35" si="17">IF(OR(C22=0, E22=0), 0, (D22*1000)/(1000/(C22*E22)))</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="166"/>
+      <c r="I22" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="J22" s="53">
+        <f>J6</f>
+        <v>1</v>
+      </c>
+      <c r="K22" s="53">
+        <v>14.006</v>
+      </c>
+      <c r="L22" s="53">
+        <f>L6</f>
+        <v>0.5</v>
+      </c>
+      <c r="M22" s="54">
+        <f>IF(OR(J22=0, L22=0), 0, (K22*1000)/(1000/(J22*L22)))</f>
+        <v>7.0030000000000001</v>
+      </c>
+      <c r="N22" s="166"/>
+      <c r="P22" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q22" s="53">
+        <f>Q6</f>
+        <v>1</v>
+      </c>
+      <c r="R22" s="53">
+        <v>14.006</v>
+      </c>
+      <c r="S22" s="53">
+        <f>S6</f>
+        <v>1</v>
+      </c>
+      <c r="T22" s="54">
+        <f>IF(OR(Q22=0,S22=0),0,(R22*1000)/(1000/(Q22*S22)))</f>
+        <v>14.006</v>
+      </c>
+      <c r="U22" s="166"/>
+      <c r="W22" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="X22" s="53">
+        <f>X6</f>
+        <v>1</v>
+      </c>
+      <c r="Y22" s="53">
+        <v>14.006</v>
+      </c>
+      <c r="Z22" s="53">
+        <f>Z6</f>
+        <v>2</v>
+      </c>
+      <c r="AA22" s="54">
+        <f>IF(OR(X22=0,Z22=0),0,(Y22*1000)/(1000/(X22*Z22)))</f>
+        <v>28.012</v>
+      </c>
+      <c r="AB22" s="166"/>
+      <c r="AD22" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE22" s="73" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF22" s="74" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B23" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="24">
+        <f>C6</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="24">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="E23" s="24">
+        <f>E6</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="166"/>
+      <c r="I23" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="J23" s="24">
+        <f>J6</f>
+        <v>1</v>
+      </c>
+      <c r="K23" s="24">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="L23" s="24">
+        <f>L6</f>
+        <v>0.5</v>
+      </c>
+      <c r="M23" s="35">
+        <f t="shared" ref="M23:M35" si="18">IF(OR(J23=0, L23=0), 0, (K23*1000)/(1000/(J23*L23)))</f>
+        <v>15.48685</v>
+      </c>
+      <c r="N23" s="166"/>
+      <c r="P23" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q23" s="24">
+        <f>Q6</f>
+        <v>1</v>
+      </c>
+      <c r="R23" s="24">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="S23" s="24">
+        <f>S6</f>
+        <v>1</v>
+      </c>
+      <c r="T23" s="35">
+        <f t="shared" ref="T23:T35" si="19">IF(OR(Q23=0,S23=0),0,(R23*1000)/(1000/(Q23*S23)))</f>
+        <v>30.973700000000001</v>
+      </c>
+      <c r="U23" s="166"/>
+      <c r="W23" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="X23" s="24">
+        <f>X6</f>
+        <v>1</v>
+      </c>
+      <c r="Y23" s="24">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="Z23" s="24">
+        <f>Z6</f>
+        <v>2</v>
+      </c>
+      <c r="AA23" s="35">
+        <f t="shared" ref="AA23:AA35" si="20">IF(OR(X23=0,Z23=0),0,(Y23*1000)/(1000/(X23*Z23)))</f>
+        <v>61.947400000000002</v>
+      </c>
+      <c r="AB23" s="166"/>
+      <c r="AD23" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE23" s="80" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF23" s="81"/>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B24" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="24">
+        <f>C7</f>
+        <v>2</v>
+      </c>
+      <c r="D24" s="24">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="E24" s="24">
+        <f>E7</f>
+        <v>2</v>
+      </c>
+      <c r="F24" s="35">
+        <f t="shared" si="17"/>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="G24" s="166"/>
+      <c r="I24" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="J24" s="24">
+        <f>J7</f>
+        <v>2</v>
+      </c>
+      <c r="K24" s="24">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="L24" s="24">
+        <f>L7</f>
+        <v>2</v>
+      </c>
+      <c r="M24" s="35">
+        <f t="shared" si="18"/>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="N24" s="166"/>
+      <c r="P24" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q24" s="24">
+        <f>Q7</f>
+        <v>2</v>
+      </c>
+      <c r="R24" s="24">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="S24" s="24">
+        <f>S7</f>
+        <v>2</v>
+      </c>
+      <c r="T24" s="35">
+        <f t="shared" si="19"/>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="U24" s="166"/>
+      <c r="W24" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="X24" s="24">
+        <f>X7</f>
+        <v>2</v>
+      </c>
+      <c r="Y24" s="24">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="Z24" s="24">
+        <f>Z7</f>
+        <v>2</v>
+      </c>
+      <c r="AA24" s="35">
+        <f t="shared" si="20"/>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="AB24" s="166"/>
+      <c r="AD24" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE24" s="83" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF24" s="84" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B25" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="24">
+        <f>C7</f>
+        <v>2</v>
+      </c>
+      <c r="D25" s="24">
+        <v>14.006</v>
+      </c>
+      <c r="E25" s="24">
+        <f>E7</f>
+        <v>2</v>
+      </c>
+      <c r="F25" s="35">
+        <f t="shared" si="17"/>
+        <v>56.024000000000001</v>
+      </c>
+      <c r="G25" s="166"/>
+      <c r="I25" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="J25" s="24">
+        <f>J7</f>
+        <v>2</v>
+      </c>
+      <c r="K25" s="24">
+        <v>14.006</v>
+      </c>
+      <c r="L25" s="24">
+        <f>L7</f>
+        <v>2</v>
+      </c>
+      <c r="M25" s="35">
+        <f t="shared" si="18"/>
+        <v>56.024000000000001</v>
+      </c>
+      <c r="N25" s="166"/>
+      <c r="P25" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q25" s="24">
+        <f>Q7</f>
+        <v>2</v>
+      </c>
+      <c r="R25" s="24">
+        <v>14.006</v>
+      </c>
+      <c r="S25" s="24">
+        <f>S7</f>
+        <v>2</v>
+      </c>
+      <c r="T25" s="35">
+        <f t="shared" si="19"/>
+        <v>56.024000000000001</v>
+      </c>
+      <c r="U25" s="166"/>
+      <c r="W25" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="X25" s="24">
+        <f>X7</f>
+        <v>2</v>
+      </c>
+      <c r="Y25" s="24">
+        <v>14.006</v>
+      </c>
+      <c r="Z25" s="24">
+        <f>Z7</f>
+        <v>2</v>
+      </c>
+      <c r="AA25" s="35">
+        <f t="shared" si="20"/>
+        <v>56.024000000000001</v>
+      </c>
+      <c r="AB25" s="166"/>
+      <c r="AD25" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE25" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF25" s="87" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B26" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="24">
+        <f>C8</f>
+        <v>2</v>
+      </c>
+      <c r="D26" s="24">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="E26" s="24">
+        <f>E8</f>
+        <v>1.5</v>
+      </c>
+      <c r="F26" s="35">
+        <f t="shared" si="17"/>
+        <v>120.23400000000001</v>
+      </c>
+      <c r="G26" s="166"/>
+      <c r="I26" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="J26" s="24">
+        <f>J8</f>
+        <v>2</v>
+      </c>
+      <c r="K26" s="24">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="L26" s="24">
+        <f>L8</f>
+        <v>1.5</v>
+      </c>
+      <c r="M26" s="35">
+        <f t="shared" si="18"/>
+        <v>120.23400000000001</v>
+      </c>
+      <c r="N26" s="166"/>
+      <c r="P26" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q26" s="24">
+        <f>Q8</f>
+        <v>2</v>
+      </c>
+      <c r="R26" s="24">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="S26" s="24">
+        <f>S8</f>
+        <v>1.25</v>
+      </c>
+      <c r="T26" s="35">
+        <f t="shared" si="19"/>
+        <v>100.19499999999999</v>
+      </c>
+      <c r="U26" s="166"/>
+      <c r="W26" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="X26" s="24">
+        <f>X8</f>
+        <v>2</v>
+      </c>
+      <c r="Y26" s="24">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="Z26" s="24">
+        <f>Z8</f>
+        <v>1.5</v>
+      </c>
+      <c r="AA26" s="35">
+        <f t="shared" si="20"/>
+        <v>120.23400000000001</v>
+      </c>
+      <c r="AB26" s="166"/>
+      <c r="AD26" s="88" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE26" s="89" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF26" s="90" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B27" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="24">
+        <f>C8</f>
+        <v>2</v>
+      </c>
+      <c r="D27" s="24">
+        <v>28.012</v>
+      </c>
+      <c r="E27" s="24">
+        <f>E8</f>
+        <v>1.5</v>
+      </c>
+      <c r="F27" s="35">
+        <f t="shared" si="17"/>
+        <v>84.036000000000001</v>
+      </c>
+      <c r="G27" s="166"/>
+      <c r="I27" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="J27" s="24">
+        <f>J8</f>
+        <v>2</v>
+      </c>
+      <c r="K27" s="24">
+        <v>28.012</v>
+      </c>
+      <c r="L27" s="24">
+        <f>L8</f>
+        <v>1.5</v>
+      </c>
+      <c r="M27" s="35">
+        <f t="shared" si="18"/>
+        <v>84.036000000000001</v>
+      </c>
+      <c r="N27" s="166"/>
+      <c r="P27" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q27" s="24">
+        <f>Q8</f>
+        <v>2</v>
+      </c>
+      <c r="R27" s="24">
+        <v>28.012</v>
+      </c>
+      <c r="S27" s="24">
+        <f>S8</f>
+        <v>1.25</v>
+      </c>
+      <c r="T27" s="35">
+        <f t="shared" si="19"/>
+        <v>70.03</v>
+      </c>
+      <c r="U27" s="166"/>
+      <c r="W27" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="X27" s="24">
+        <f>X8</f>
+        <v>2</v>
+      </c>
+      <c r="Y27" s="24">
+        <v>28.012</v>
+      </c>
+      <c r="Z27" s="24">
+        <f>Z8</f>
+        <v>1.5</v>
+      </c>
+      <c r="AA27" s="35">
+        <f t="shared" si="20"/>
+        <v>84.036000000000001</v>
+      </c>
+      <c r="AB27" s="166"/>
+      <c r="AD27" s="23"/>
+      <c r="AE27" s="75"/>
+      <c r="AF27" s="11"/>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B28" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="24">
+        <f>C9</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="24">
+        <v>28.012</v>
+      </c>
+      <c r="E28" s="24">
+        <f>E9</f>
+        <v>2.5</v>
+      </c>
+      <c r="F28" s="35">
+        <f>IF(OR(C28=0, E28=0), 0, (D28*1000)/(1000/(C28*E28)))</f>
+        <v>70.03</v>
+      </c>
+      <c r="G28" s="166"/>
+      <c r="I28" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="J28" s="24">
+        <f>J9</f>
+        <v>1</v>
+      </c>
+      <c r="K28" s="24">
+        <v>28.012</v>
+      </c>
+      <c r="L28" s="24">
+        <f>L9</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M28" s="35">
+        <f t="shared" si="18"/>
+        <v>64.427599999999998</v>
+      </c>
+      <c r="N28" s="166"/>
+      <c r="P28" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q28" s="24">
+        <f>Q9</f>
+        <v>1</v>
+      </c>
+      <c r="R28" s="24">
+        <v>28.012</v>
+      </c>
+      <c r="S28" s="24">
+        <f>S9</f>
+        <v>2.5</v>
+      </c>
+      <c r="T28" s="35">
+        <f t="shared" si="19"/>
+        <v>70.03</v>
+      </c>
+      <c r="U28" s="166"/>
+      <c r="W28" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="X28" s="24">
+        <f>X9</f>
+        <v>1</v>
+      </c>
+      <c r="Y28" s="24">
+        <v>28.012</v>
+      </c>
+      <c r="Z28" s="24">
+        <f>Z9</f>
+        <v>1.5</v>
+      </c>
+      <c r="AA28" s="35">
+        <f>IF(OR(X28=0,Z28=0),0,(Y28*1000)/(1000/(X28*Z28)))</f>
+        <v>42.018000000000001</v>
+      </c>
+      <c r="AB28" s="166"/>
+      <c r="AD28" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE28" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF28" s="93" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B29" s="95" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="24">
+        <f>C13</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="24">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="E29" s="24">
+        <f>E13</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="166"/>
+      <c r="I29" s="95" t="s">
+        <v>83</v>
+      </c>
+      <c r="J29" s="24">
+        <f>J13</f>
+        <v>1</v>
+      </c>
+      <c r="K29" s="24">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="L29" s="24">
+        <f>L13</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="35">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="166"/>
+      <c r="P29" s="95" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q29" s="24">
+        <f>Q13</f>
+        <v>1</v>
+      </c>
+      <c r="R29" s="24">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="S29" s="24">
+        <f>S13</f>
+        <v>0</v>
+      </c>
+      <c r="T29" s="35">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U29" s="166"/>
+      <c r="W29" s="95" t="s">
+        <v>83</v>
+      </c>
+      <c r="X29" s="24">
+        <f>X13</f>
+        <v>1</v>
+      </c>
+      <c r="Y29" s="24">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="Z29" s="24">
+        <f>Z13</f>
+        <v>0</v>
+      </c>
+      <c r="AA29" s="35">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AB29" s="166"/>
+      <c r="AD29" s="99" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE29" s="100" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF29" s="101" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B30" s="95" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="24">
+        <f>C13</f>
+        <v>1</v>
+      </c>
+      <c r="D30" s="24">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="E30" s="24">
+        <f>E13</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="166"/>
+      <c r="I30" s="95" t="s">
+        <v>84</v>
+      </c>
+      <c r="J30" s="24">
+        <f>J13</f>
+        <v>1</v>
+      </c>
+      <c r="K30" s="24">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="L30" s="24">
+        <f>L13</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="35">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="166"/>
+      <c r="P30" s="95" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q30" s="24">
+        <f>Q13</f>
+        <v>1</v>
+      </c>
+      <c r="R30" s="24">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="S30" s="24">
+        <f>S13</f>
+        <v>0</v>
+      </c>
+      <c r="T30" s="35">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U30" s="166"/>
+      <c r="W30" s="95" t="s">
+        <v>84</v>
+      </c>
+      <c r="X30" s="24">
+        <f>X13</f>
+        <v>1</v>
+      </c>
+      <c r="Y30" s="24">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="Z30" s="24">
+        <f>Z13</f>
+        <v>0</v>
+      </c>
+      <c r="AA30" s="35">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AB30" s="166"/>
+      <c r="AD30" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE30" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF30" s="104" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B31" s="96" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="24">
+        <f>C14</f>
+        <v>1</v>
+      </c>
+      <c r="D31" s="24">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="E31" s="24">
+        <f>E14</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="166"/>
+      <c r="I31" s="96" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="24">
+        <f>J14</f>
+        <v>1</v>
+      </c>
+      <c r="K31" s="24">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="L31" s="24">
+        <f>L14</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="35">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="166"/>
+      <c r="P31" s="96" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q31" s="24">
+        <f>Q14</f>
+        <v>1</v>
+      </c>
+      <c r="R31" s="24">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="S31" s="24">
+        <f>S14</f>
+        <v>0</v>
+      </c>
+      <c r="T31" s="35">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U31" s="166"/>
+      <c r="W31" s="96" t="s">
+        <v>11</v>
+      </c>
+      <c r="X31" s="24">
+        <f>X14</f>
+        <v>1</v>
+      </c>
+      <c r="Y31" s="24">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="Z31" s="24">
+        <f>Z14</f>
+        <v>0</v>
+      </c>
+      <c r="AA31" s="35">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="166"/>
+      <c r="AD31" s="105" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE31" s="106" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF31" s="107" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B32" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="24">
+        <f>C14</f>
+        <v>1</v>
+      </c>
+      <c r="D32" s="24">
+        <v>35.453000000000003</v>
+      </c>
+      <c r="E32" s="24">
+        <f>E14</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="166"/>
+      <c r="I32" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="24">
+        <f>J14</f>
+        <v>1</v>
+      </c>
+      <c r="K32" s="24">
+        <v>35.453000000000003</v>
+      </c>
+      <c r="L32" s="24">
+        <f>L14</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="35">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="166"/>
+      <c r="P32" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q32" s="24">
+        <f>Q14</f>
+        <v>1</v>
+      </c>
+      <c r="R32" s="24">
+        <v>35.453000000000003</v>
+      </c>
+      <c r="S32" s="24">
+        <f>S14</f>
+        <v>0</v>
+      </c>
+      <c r="T32" s="35">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="U32" s="166"/>
+      <c r="W32" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="X32" s="24">
+        <f>X14</f>
+        <v>1</v>
+      </c>
+      <c r="Y32" s="24">
+        <v>35.453000000000003</v>
+      </c>
+      <c r="Z32" s="24">
+        <f>Z14</f>
+        <v>0</v>
+      </c>
+      <c r="AA32" s="35">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AB32" s="166"/>
+      <c r="AD32" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE32" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF32" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B33" s="97" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="24">
+        <f>C15</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="24">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="E33" s="24">
+        <f>E15</f>
+        <v>1</v>
+      </c>
+      <c r="F33" s="35">
+        <f t="shared" si="17"/>
+        <v>40.078000000000003</v>
+      </c>
+      <c r="G33" s="166"/>
+      <c r="I33" s="97" t="s">
+        <v>85</v>
+      </c>
+      <c r="J33" s="24">
+        <f>J15</f>
+        <v>1</v>
+      </c>
+      <c r="K33" s="24">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="L33" s="24">
+        <f>L15</f>
+        <v>1</v>
+      </c>
+      <c r="M33" s="35">
+        <f t="shared" si="18"/>
+        <v>40.078000000000003</v>
+      </c>
+      <c r="N33" s="166"/>
+      <c r="P33" s="97" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q33" s="24">
+        <f>Q15</f>
+        <v>1</v>
+      </c>
+      <c r="R33" s="24">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="S33" s="24">
+        <f>S15</f>
+        <v>1.5</v>
+      </c>
+      <c r="T33" s="35">
+        <f t="shared" si="19"/>
+        <v>60.117000000000004</v>
+      </c>
+      <c r="U33" s="166"/>
+      <c r="W33" s="97" t="s">
+        <v>85</v>
+      </c>
+      <c r="X33" s="24">
+        <f>X15</f>
+        <v>1</v>
+      </c>
+      <c r="Y33" s="24">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="Z33" s="24">
+        <f>Z15</f>
+        <v>1</v>
+      </c>
+      <c r="AA33" s="35">
+        <f t="shared" si="20"/>
+        <v>40.078000000000003</v>
+      </c>
+      <c r="AB33" s="166"/>
+      <c r="AD33" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE33" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF33" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B34" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="24">
+        <f>C16</f>
+        <v>2</v>
+      </c>
+      <c r="D34" s="24">
+        <v>24.305</v>
+      </c>
+      <c r="E34" s="24">
+        <f>E16</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="35">
+        <f t="shared" si="17"/>
+        <v>48.61</v>
+      </c>
+      <c r="G34" s="166"/>
+      <c r="I34" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="J34" s="24">
+        <f>J16</f>
+        <v>2</v>
+      </c>
+      <c r="K34" s="24">
+        <v>24.305</v>
+      </c>
+      <c r="L34" s="24">
+        <f>L16</f>
+        <v>1</v>
+      </c>
+      <c r="M34" s="35">
+        <f t="shared" si="18"/>
+        <v>48.61</v>
+      </c>
+      <c r="N34" s="166"/>
+      <c r="P34" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q34" s="24">
+        <f>Q16</f>
+        <v>2</v>
+      </c>
+      <c r="R34" s="24">
+        <v>24.305</v>
+      </c>
+      <c r="S34" s="24">
+        <f>S16</f>
+        <v>1</v>
+      </c>
+      <c r="T34" s="35">
+        <f t="shared" si="19"/>
+        <v>48.61</v>
+      </c>
+      <c r="U34" s="166"/>
+      <c r="W34" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="X34" s="24">
+        <f>X16</f>
+        <v>2</v>
+      </c>
+      <c r="Y34" s="24">
+        <v>24.305</v>
+      </c>
+      <c r="Z34" s="24">
+        <f>Z16</f>
+        <v>1</v>
+      </c>
+      <c r="AA34" s="35">
+        <f t="shared" si="20"/>
+        <v>48.61</v>
+      </c>
+      <c r="AB34" s="166"/>
+      <c r="AD34" s="23"/>
+      <c r="AE34" s="75"/>
+      <c r="AF34" s="11"/>
+    </row>
+    <row r="35" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="24">
+        <f>C16</f>
+        <v>2</v>
+      </c>
+      <c r="D35" s="24">
+        <v>32.064999999999998</v>
+      </c>
+      <c r="E35" s="24">
+        <f>E16</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="35">
+        <f t="shared" si="17"/>
+        <v>64.13</v>
+      </c>
+      <c r="G35" s="166"/>
+      <c r="I35" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="J35" s="24">
+        <f>J16</f>
+        <v>2</v>
+      </c>
+      <c r="K35" s="24">
+        <v>32.064999999999998</v>
+      </c>
+      <c r="L35" s="24">
+        <f>L16</f>
+        <v>1</v>
+      </c>
+      <c r="M35" s="35">
+        <f t="shared" si="18"/>
+        <v>64.13</v>
+      </c>
+      <c r="N35" s="166"/>
+      <c r="P35" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q35" s="24">
+        <f>Q16</f>
+        <v>2</v>
+      </c>
+      <c r="R35" s="24">
+        <v>32.064999999999998</v>
+      </c>
+      <c r="S35" s="24">
+        <f>S16</f>
+        <v>1</v>
+      </c>
+      <c r="T35" s="35">
+        <f t="shared" si="19"/>
+        <v>64.13</v>
+      </c>
+      <c r="U35" s="166"/>
+      <c r="W35" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="X35" s="24">
+        <f>X16</f>
+        <v>2</v>
+      </c>
+      <c r="Y35" s="24">
+        <v>32.064999999999998</v>
+      </c>
+      <c r="Z35" s="24">
+        <f>Z16</f>
+        <v>1</v>
+      </c>
+      <c r="AA35" s="35">
+        <f t="shared" si="20"/>
+        <v>64.13</v>
+      </c>
+      <c r="AB35" s="166"/>
+      <c r="AD35" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE35" s="5">
+        <v>30.974</v>
+      </c>
+      <c r="AF35" s="6"/>
+    </row>
+    <row r="36" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="33"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="166"/>
+      <c r="I36" s="33"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="166"/>
+      <c r="P36" s="33"/>
+      <c r="T36" s="36"/>
+      <c r="U36" s="166"/>
+      <c r="W36" s="33"/>
+      <c r="AA36" s="36"/>
+      <c r="AB36" s="166"/>
+    </row>
+    <row r="37" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B37" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="45"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="167"/>
+      <c r="I37" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="45"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="52"/>
+      <c r="N37" s="168"/>
+      <c r="P37" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q37" s="45"/>
+      <c r="R37" s="46"/>
+      <c r="S37" s="46"/>
+      <c r="T37" s="52"/>
+      <c r="U37" s="168"/>
+      <c r="W37" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="X37" s="45"/>
+      <c r="Y37" s="46"/>
+      <c r="Z37" s="46"/>
+      <c r="AA37" s="52"/>
+      <c r="AB37" s="168"/>
+    </row>
+    <row r="38" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="50"/>
+      <c r="E38" s="146" t="s">
+        <v>103</v>
+      </c>
+      <c r="F38" s="51"/>
+      <c r="G38" s="168"/>
+      <c r="I38" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="K38" s="50"/>
+      <c r="L38" s="146" t="s">
+        <v>103</v>
+      </c>
+      <c r="M38" s="51"/>
+      <c r="N38" s="168"/>
+      <c r="P38" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q38" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="R38" s="50"/>
+      <c r="S38" s="146" t="s">
+        <v>103</v>
+      </c>
+      <c r="T38" s="51"/>
+      <c r="U38" s="168"/>
+      <c r="W38" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="X38" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y38" s="50"/>
+      <c r="Z38" s="146" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA38" s="51"/>
+      <c r="AB38" s="168"/>
+    </row>
+    <row r="39" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B39" s="158" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="150">
+        <f>SUM(F22,F25,F27,F28)</f>
+        <v>210.09</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="37">
+        <f>C48-C39</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="34"/>
+      <c r="G39" s="165"/>
+      <c r="I39" s="115" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="150">
+        <f>SUM(M22,M25,M27,M28)</f>
+        <v>211.49059999999997</v>
+      </c>
+      <c r="L39" s="37">
+        <f>C48-J39</f>
+        <v>-1.4005999999999688</v>
+      </c>
+      <c r="M39" s="34"/>
+      <c r="N39" s="165"/>
+      <c r="P39" s="115" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q39" s="61">
+        <f>SUM(T22,T25,T27,T28)</f>
+        <v>210.09</v>
+      </c>
+      <c r="S39" s="147">
+        <f>Q39-C48</f>
+        <v>0</v>
+      </c>
+      <c r="T39" s="34"/>
+      <c r="U39" s="165"/>
+      <c r="W39" s="115" t="s">
+        <v>15</v>
+      </c>
+      <c r="X39" s="61">
+        <f>SUM(AA22,AA25,AA27,AA28)</f>
+        <v>210.09</v>
+      </c>
+      <c r="Z39" s="37">
+        <f>C48-X39</f>
+        <v>0</v>
+      </c>
+      <c r="AA39" s="34"/>
+      <c r="AB39" s="165"/>
+    </row>
+    <row r="40" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B40" s="159" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="24">
+        <f>SUM(F23,F30)</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="37">
+        <f t="shared" ref="E40:E44" si="21">C49-C40</f>
+        <v>30.973700000000001</v>
+      </c>
+      <c r="F40" s="34"/>
+      <c r="G40" s="165"/>
+      <c r="I40" s="116" t="s">
+        <v>16</v>
+      </c>
+      <c r="J40" s="24">
+        <f>SUM(M23,M30)</f>
+        <v>15.48685</v>
+      </c>
+      <c r="L40" s="37">
+        <f t="shared" ref="L40:L44" si="22">C49-J40</f>
+        <v>15.48685</v>
+      </c>
+      <c r="M40" s="34"/>
+      <c r="N40" s="165"/>
+      <c r="P40" s="116" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q40" s="24">
+        <f>SUM(T23,T30)</f>
+        <v>30.973700000000001</v>
+      </c>
+      <c r="S40" s="147">
+        <f t="shared" ref="S40:S44" si="23">Q40-C49</f>
+        <v>0</v>
+      </c>
+      <c r="T40" s="34"/>
+      <c r="U40" s="165"/>
+      <c r="W40" s="116" t="s">
+        <v>16</v>
+      </c>
+      <c r="X40" s="24">
+        <f>SUM(AA23,AA30)</f>
+        <v>61.947400000000002</v>
+      </c>
+      <c r="Z40" s="37">
+        <f t="shared" ref="Z40:Z44" si="24">C49-X40</f>
+        <v>-30.973700000000001</v>
+      </c>
+      <c r="AA40" s="34"/>
+      <c r="AB40" s="165"/>
+    </row>
+    <row r="41" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B41" s="159" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="148">
+        <f>SUM(F24,F29,F31)</f>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="E41" s="37">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="34"/>
+      <c r="G41" s="165"/>
+      <c r="I41" s="116" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="59">
+        <f>SUM(M24,M29,M31)</f>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="L41" s="37">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="34"/>
+      <c r="N41" s="165"/>
+      <c r="P41" s="116" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q41" s="59">
+        <f>SUM(T24,T29,T31)</f>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="S41" s="147">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T41" s="34"/>
+      <c r="U41" s="165"/>
+      <c r="W41" s="116" t="s">
+        <v>17</v>
+      </c>
+      <c r="X41" s="59">
+        <f>SUM(AA24,AA29,AA31)</f>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="Z41" s="37">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AA41" s="34"/>
+      <c r="AB41" s="165"/>
+    </row>
+    <row r="42" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B42" s="159" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="59">
+        <f>F26+F33</f>
+        <v>160.31200000000001</v>
+      </c>
+      <c r="E42" s="37">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="34"/>
+      <c r="G42" s="165"/>
+      <c r="I42" s="116" t="s">
+        <v>18</v>
+      </c>
+      <c r="J42" s="59">
+        <f>M26+M33</f>
+        <v>160.31200000000001</v>
+      </c>
+      <c r="L42" s="37">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="34"/>
+      <c r="N42" s="165"/>
+      <c r="P42" s="116" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q42" s="59">
+        <f>T26+T33</f>
+        <v>160.31200000000001</v>
+      </c>
+      <c r="S42" s="147">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T42" s="34"/>
+      <c r="U42" s="165"/>
+      <c r="W42" s="116" t="s">
+        <v>18</v>
+      </c>
+      <c r="X42" s="59">
+        <f>AA26+AA33</f>
+        <v>160.31200000000001</v>
+      </c>
+      <c r="Z42" s="37">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AA42" s="34"/>
+      <c r="AB42" s="165"/>
+    </row>
+    <row r="43" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B43" s="116" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="59">
+        <f>F34</f>
+        <v>48.61</v>
+      </c>
+      <c r="E43" s="37">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="34"/>
+      <c r="G43" s="165"/>
+      <c r="I43" s="116" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" s="59">
+        <f>M34</f>
+        <v>48.61</v>
+      </c>
+      <c r="L43" s="37">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="34"/>
+      <c r="N43" s="165"/>
+      <c r="P43" s="116" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q43" s="59">
+        <f>T34</f>
+        <v>48.61</v>
+      </c>
+      <c r="S43" s="147">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T43" s="34"/>
+      <c r="U43" s="165"/>
+      <c r="W43" s="116" t="s">
+        <v>19</v>
+      </c>
+      <c r="X43" s="59">
+        <f>AA34</f>
+        <v>48.61</v>
+      </c>
+      <c r="Z43" s="37">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AA43" s="34"/>
+      <c r="AB43" s="165"/>
+    </row>
+    <row r="44" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="117" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="60">
+        <f>F35</f>
+        <v>64.13</v>
+      </c>
+      <c r="D44" s="38"/>
+      <c r="E44" s="37">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="40"/>
+      <c r="G44" s="165"/>
+      <c r="I44" s="117" t="s">
+        <v>20</v>
+      </c>
+      <c r="J44" s="60">
+        <f>M35</f>
+        <v>64.13</v>
+      </c>
+      <c r="K44" s="38"/>
+      <c r="L44" s="37">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="40"/>
+      <c r="N44" s="165"/>
+      <c r="P44" s="117" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q44" s="60">
+        <f>T35</f>
+        <v>64.13</v>
+      </c>
+      <c r="R44" s="38"/>
+      <c r="S44" s="147">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T44" s="40"/>
+      <c r="U44" s="165"/>
+      <c r="W44" s="117" t="s">
+        <v>20</v>
+      </c>
+      <c r="X44" s="60">
+        <f>AA35</f>
+        <v>64.13</v>
+      </c>
+      <c r="Y44" s="38"/>
+      <c r="Z44" s="37">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AA44" s="40"/>
+      <c r="AB44" s="165"/>
+    </row>
+    <row r="47" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B47" s="145" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48">
+        <v>210.09</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49">
+        <v>30.973700000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50">
+        <v>156.37719999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51">
+        <v>160.31200000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52">
+        <v>48.61</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53">
+        <v>64.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E39:E44 L39:L44 S39:S44 Z39:Z44">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
+      <formula>-2</formula>
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="33" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5402332-2850-4AF6-A36B-1E4FE336591B}">
   <dimension ref="B1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
added greenhouse layout & log updates
</commit_message>
<xml_diff>
--- a/meta_data/hoaglands_recipes_p_v1.xlsx
+++ b/meta_data/hoaglands_recipes_p_v1.xlsx
@@ -8,11 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monik\Documents\git\2025_g34p\meta_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EA2F98-EF35-407E-800D-C8830B864085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B94397-F169-4442-83D5-F8CE85E2AF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{672A70A4-BEEB-4E9F-898A-72ED4A72F9C3}"/>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{5A275A07-A470-45D3-A544-9A609AEF5A01}"/>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="7" xr2:uid="{80806F84-9466-4FB7-909E-FA04A69E8008}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{5A275A07-A470-45D3-A544-9A609AEF5A01}"/>
   </bookViews>
   <sheets>
     <sheet name="recipes_v1" sheetId="4" r:id="rId1"/>
@@ -22,7 +20,8 @@
     <sheet name="recipes_v5" sheetId="9" r:id="rId5"/>
     <sheet name="recipes_v6" sheetId="10" r:id="rId6"/>
     <sheet name="recipe_winners" sheetId="13" r:id="rId7"/>
-    <sheet name="pH_notes" sheetId="12" r:id="rId8"/>
+    <sheet name="recipe_final" sheetId="14" r:id="rId8"/>
+    <sheet name="pH_notes" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2384" uniqueCount="139">
   <si>
     <t>Primary N addition compounds</t>
   </si>
@@ -1844,6 +1843,39 @@
   <si>
     <t>(recipe v3)</t>
   </si>
+  <si>
+    <t>mL for 20 L</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
 </sst>
 </file>
 
@@ -2469,7 +2501,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2640,16 +2672,35 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3056,11 +3107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C991C1-A1AF-4EC8-80EB-A4FE0F14FB5F}">
   <dimension ref="B1:AB44"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5738,12 +5785,8 @@
   <dimension ref="B1:AF53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8821,7 +8864,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E39:E44 L39:L44 S39:S44 Z39:Z44">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="between">
       <formula>-2</formula>
       <formula>2</formula>
     </cfRule>
@@ -8838,13 +8881,7 @@
   </sheetPr>
   <dimension ref="B1:AF53"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-    <sheetView topLeftCell="G1" workbookViewId="2">
-      <selection activeCell="S13" sqref="S13:S18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11922,7 +11959,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E39:E44 L39:L44 S39:S44 Z39:Z44">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="between">
       <formula>-2</formula>
       <formula>2</formula>
     </cfRule>
@@ -11939,11 +11976,7 @@
   </sheetPr>
   <dimension ref="B1:AF53"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:U44"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15022,7 +15055,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E39:E44 L39:L44 S39:S44 Z39:Z44">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="between">
       <formula>-2</formula>
       <formula>2</formula>
     </cfRule>
@@ -15039,11 +15072,7 @@
   </sheetPr>
   <dimension ref="B1:AF53"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:U44"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18117,7 +18146,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E39:E44 L39:L44 S39:S44 Z39:Z44">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
       <formula>-2</formula>
       <formula>2</formula>
     </cfRule>
@@ -18134,13 +18163,7 @@
   </sheetPr>
   <dimension ref="B1:AF53"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="W26" sqref="W26"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-    <sheetView topLeftCell="N18" workbookViewId="2">
-      <selection activeCell="W39" sqref="W39:X44"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21218,7 +21241,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E39:E44 L39:L44 S39:S44 Z39:Z44">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>-2</formula>
       <formula>2</formula>
     </cfRule>
@@ -21235,11 +21258,7 @@
   </sheetPr>
   <dimension ref="B1:AF53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q37" sqref="Q37"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21508,7 +21527,7 @@
       <c r="D6" s="51">
         <v>115.3</v>
       </c>
-      <c r="E6" s="138">
+      <c r="E6" s="51">
         <v>0</v>
       </c>
       <c r="F6" s="53">
@@ -21528,7 +21547,7 @@
       <c r="K6" s="51">
         <v>115.3</v>
       </c>
-      <c r="L6" s="138">
+      <c r="L6" s="51">
         <v>0.5</v>
       </c>
       <c r="M6" s="53">
@@ -21548,7 +21567,7 @@
       <c r="R6" s="51">
         <v>115.3</v>
       </c>
-      <c r="S6" s="138">
+      <c r="S6" s="51">
         <v>1</v>
       </c>
       <c r="T6" s="53">
@@ -21600,7 +21619,7 @@
       <c r="D7" s="22">
         <v>101.1</v>
       </c>
-      <c r="E7" s="139">
+      <c r="E7" s="22">
         <v>2</v>
       </c>
       <c r="F7" s="30">
@@ -21620,7 +21639,7 @@
       <c r="K7" s="22">
         <v>101.1</v>
       </c>
-      <c r="L7" s="139">
+      <c r="L7" s="22">
         <v>2</v>
       </c>
       <c r="M7" s="30">
@@ -21640,7 +21659,7 @@
       <c r="R7" s="22">
         <v>101.1</v>
       </c>
-      <c r="S7" s="139">
+      <c r="S7" s="22">
         <v>2</v>
       </c>
       <c r="T7" s="30">
@@ -21691,7 +21710,7 @@
       <c r="D8" s="22">
         <v>164.08799999999999</v>
       </c>
-      <c r="E8" s="139">
+      <c r="E8" s="22">
         <v>2</v>
       </c>
       <c r="F8" s="30">
@@ -21711,7 +21730,7 @@
       <c r="K8" s="22">
         <v>164.08799999999999</v>
       </c>
-      <c r="L8" s="139">
+      <c r="L8" s="22">
         <v>1.75</v>
       </c>
       <c r="M8" s="30">
@@ -21731,7 +21750,7 @@
       <c r="R8" s="22">
         <v>164.08799999999999</v>
       </c>
-      <c r="S8" s="139">
+      <c r="S8" s="22">
         <v>1.5</v>
       </c>
       <c r="T8" s="30">
@@ -21783,7 +21802,7 @@
       <c r="D9" s="112">
         <v>80.043000000000006</v>
       </c>
-      <c r="E9" s="139">
+      <c r="E9" s="22">
         <v>1.5</v>
       </c>
       <c r="F9" s="30">
@@ -21803,7 +21822,7 @@
       <c r="K9" s="22">
         <v>80.043000000000006</v>
       </c>
-      <c r="L9" s="139">
+      <c r="L9" s="22">
         <v>1.75</v>
       </c>
       <c r="M9" s="30">
@@ -21823,7 +21842,7 @@
       <c r="R9" s="22">
         <v>80.043000000000006</v>
       </c>
-      <c r="S9" s="139">
+      <c r="S9" s="22">
         <v>2</v>
       </c>
       <c r="T9" s="30">
@@ -21868,10 +21887,8 @@
       <c r="B10" s="31"/>
       <c r="F10" s="32"/>
       <c r="I10" s="31"/>
-      <c r="L10" s="140"/>
       <c r="M10" s="32"/>
       <c r="P10" s="31"/>
-      <c r="S10" s="140"/>
       <c r="T10" s="32"/>
       <c r="W10" s="31"/>
       <c r="AA10" s="32"/>
@@ -22020,7 +22037,7 @@
       <c r="D13" s="51">
         <v>136.08600000000001</v>
       </c>
-      <c r="E13" s="138">
+      <c r="E13" s="51">
         <v>0</v>
       </c>
       <c r="F13" s="52">
@@ -22040,7 +22057,7 @@
       <c r="K13" s="51">
         <v>136.08600000000001</v>
       </c>
-      <c r="L13" s="138">
+      <c r="L13" s="51">
         <v>0</v>
       </c>
       <c r="M13" s="52">
@@ -22060,7 +22077,7 @@
       <c r="R13" s="51">
         <v>136.08600000000001</v>
       </c>
-      <c r="S13" s="138">
+      <c r="S13" s="51">
         <v>0</v>
       </c>
       <c r="T13" s="52">
@@ -22110,7 +22127,7 @@
       <c r="D14" s="22">
         <v>74.555000000000007</v>
       </c>
-      <c r="E14" s="139">
+      <c r="E14" s="22">
         <v>0</v>
       </c>
       <c r="F14" s="33">
@@ -22130,7 +22147,7 @@
       <c r="K14" s="22">
         <v>74.555000000000007</v>
       </c>
-      <c r="L14" s="139">
+      <c r="L14" s="22">
         <v>0</v>
       </c>
       <c r="M14" s="33">
@@ -22150,7 +22167,7 @@
       <c r="R14" s="22">
         <v>74.555000000000007</v>
       </c>
-      <c r="S14" s="139">
+      <c r="S14" s="22">
         <v>0</v>
       </c>
       <c r="T14" s="33">
@@ -22196,7 +22213,7 @@
       <c r="D15" s="22">
         <v>100.087</v>
       </c>
-      <c r="E15" s="139">
+      <c r="E15" s="22">
         <v>0.04</v>
       </c>
       <c r="F15" s="33">
@@ -22216,7 +22233,7 @@
       <c r="K15" s="22">
         <v>100.087</v>
       </c>
-      <c r="L15" s="139">
+      <c r="L15" s="22">
         <v>0.5</v>
       </c>
       <c r="M15" s="33">
@@ -22236,7 +22253,7 @@
       <c r="R15" s="22">
         <v>100.087</v>
       </c>
-      <c r="S15" s="139">
+      <c r="S15" s="22">
         <v>1</v>
       </c>
       <c r="T15" s="33">
@@ -22286,7 +22303,7 @@
       <c r="D16" s="22">
         <v>246.48</v>
       </c>
-      <c r="E16" s="139">
+      <c r="E16" s="22">
         <v>1</v>
       </c>
       <c r="F16" s="33">
@@ -22306,7 +22323,7 @@
       <c r="K16" s="22">
         <v>246.48</v>
       </c>
-      <c r="L16" s="139">
+      <c r="L16" s="22">
         <v>1</v>
       </c>
       <c r="M16" s="33">
@@ -22326,7 +22343,7 @@
       <c r="R16" s="22">
         <v>246.48</v>
       </c>
-      <c r="S16" s="139">
+      <c r="S16" s="22">
         <v>1</v>
       </c>
       <c r="T16" s="33">
@@ -22375,7 +22392,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="22"/>
-      <c r="E17" s="139">
+      <c r="E17" s="22">
         <v>1</v>
       </c>
       <c r="F17" s="33"/>
@@ -22390,7 +22407,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="22"/>
-      <c r="L17" s="139">
+      <c r="L17" s="22">
         <v>1</v>
       </c>
       <c r="M17" s="33"/>
@@ -22405,7 +22422,7 @@
         <v>1</v>
       </c>
       <c r="R17" s="22"/>
-      <c r="S17" s="139">
+      <c r="S17" s="22">
         <v>1</v>
       </c>
       <c r="T17" s="33">
@@ -22449,7 +22466,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="22"/>
-      <c r="E18" s="139">
+      <c r="E18" s="22">
         <v>1</v>
       </c>
       <c r="F18" s="33">
@@ -22467,7 +22484,7 @@
         <v>1</v>
       </c>
       <c r="K18" s="22"/>
-      <c r="L18" s="139">
+      <c r="L18" s="22">
         <v>1</v>
       </c>
       <c r="M18" s="33">
@@ -22485,7 +22502,7 @@
         <v>1</v>
       </c>
       <c r="R18" s="22"/>
-      <c r="S18" s="139">
+      <c r="S18" s="22">
         <v>1</v>
       </c>
       <c r="T18" s="33">
@@ -24039,7 +24056,7 @@
         <v>15.48685</v>
       </c>
       <c r="L40" s="35">
-        <f t="shared" ref="L40:L44" si="22">C49-J40</f>
+        <f>C49-J40</f>
         <v>15.48685</v>
       </c>
       <c r="M40" s="32"/>
@@ -24051,7 +24068,7 @@
         <v>30.973700000000001</v>
       </c>
       <c r="S40" s="118">
-        <f t="shared" ref="S40:S44" si="23">Q40-C49</f>
+        <f>Q40-C49</f>
         <v>0</v>
       </c>
       <c r="T40" s="32"/>
@@ -24063,7 +24080,7 @@
         <v>61.947400000000002</v>
       </c>
       <c r="Z40" s="35">
-        <f t="shared" ref="Z40:Z44" si="24">C49-X40</f>
+        <f>C49-X40</f>
         <v>-30.973700000000001</v>
       </c>
       <c r="AA40" s="32"/>
@@ -24089,7 +24106,7 @@
         <v>156.37719999999999</v>
       </c>
       <c r="L41" s="35">
-        <f t="shared" si="22"/>
+        <f>C50-J41</f>
         <v>0</v>
       </c>
       <c r="M41" s="32"/>
@@ -24101,7 +24118,7 @@
         <v>156.37719999999999</v>
       </c>
       <c r="S41" s="118">
-        <f t="shared" si="23"/>
+        <f>Q41-C50</f>
         <v>0</v>
       </c>
       <c r="T41" s="32"/>
@@ -24113,7 +24130,7 @@
         <v>156.37719999999999</v>
       </c>
       <c r="Z41" s="35">
-        <f t="shared" si="24"/>
+        <f>C50-X41</f>
         <v>0</v>
       </c>
       <c r="AA41" s="32"/>
@@ -24139,7 +24156,7 @@
         <v>160.31200000000001</v>
       </c>
       <c r="L42" s="35">
-        <f t="shared" si="22"/>
+        <f>C51-J42</f>
         <v>0</v>
       </c>
       <c r="M42" s="32"/>
@@ -24151,7 +24168,7 @@
         <v>160.31200000000001</v>
       </c>
       <c r="S42" s="118">
-        <f t="shared" si="23"/>
+        <f>Q42-C51</f>
         <v>0</v>
       </c>
       <c r="T42" s="32"/>
@@ -24163,7 +24180,7 @@
         <v>160.31199999999998</v>
       </c>
       <c r="Z42" s="35">
-        <f t="shared" si="24"/>
+        <f>C51-X42</f>
         <v>0</v>
       </c>
       <c r="AA42" s="32"/>
@@ -24189,7 +24206,7 @@
         <v>48.61</v>
       </c>
       <c r="L43" s="35">
-        <f t="shared" si="22"/>
+        <f>C52-J43</f>
         <v>0</v>
       </c>
       <c r="M43" s="32"/>
@@ -24201,7 +24218,7 @@
         <v>48.61</v>
       </c>
       <c r="S43" s="118">
-        <f t="shared" si="23"/>
+        <f>Q43-C52</f>
         <v>0</v>
       </c>
       <c r="T43" s="32"/>
@@ -24213,7 +24230,7 @@
         <v>48.61</v>
       </c>
       <c r="Z43" s="35">
-        <f t="shared" si="24"/>
+        <f>C52-X43</f>
         <v>0</v>
       </c>
       <c r="AA43" s="32"/>
@@ -24241,7 +24258,7 @@
       </c>
       <c r="K44" s="36"/>
       <c r="L44" s="35">
-        <f t="shared" si="22"/>
+        <f>C53-J44</f>
         <v>0</v>
       </c>
       <c r="M44" s="38"/>
@@ -24254,7 +24271,7 @@
       </c>
       <c r="R44" s="36"/>
       <c r="S44" s="118">
-        <f t="shared" si="23"/>
+        <f>Q44-C53</f>
         <v>0</v>
       </c>
       <c r="T44" s="38"/>
@@ -24267,7 +24284,7 @@
       </c>
       <c r="Y44" s="36"/>
       <c r="Z44" s="35">
-        <f t="shared" si="24"/>
+        <f>C53-X44</f>
         <v>0</v>
       </c>
       <c r="AA44" s="38"/>
@@ -24327,7 +24344,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E39:E44 L39:L44 S39:S44 Z39:Z44">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
       <formula>-2</formula>
       <formula>2</formula>
     </cfRule>
@@ -24338,16 +24355,3367 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C63D39-1EBA-4E78-AA53-84340A8EC12C}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:AJ53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28" style="2" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="4.85546875" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" customWidth="1"/>
+    <col min="17" max="17" width="7.140625" customWidth="1"/>
+    <col min="18" max="18" width="29.7109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="3.5703125" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" customWidth="1"/>
+    <col min="25" max="25" width="7.140625" customWidth="1"/>
+    <col min="26" max="26" width="26.85546875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="13" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.5703125" customWidth="1"/>
+    <col min="32" max="32" width="10.42578125" customWidth="1"/>
+    <col min="34" max="34" width="49" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="47.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="111"/>
+    </row>
+    <row r="2" spans="2:36" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="106" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="139"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="140"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="140"/>
+      <c r="AF2" s="27"/>
+      <c r="AH2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="9"/>
+    </row>
+    <row r="3" spans="2:36" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="26">
+        <f>C40/AI35</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="26">
+        <f>K40/AI35</f>
+        <v>0.49999515722864341</v>
+      </c>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="140"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="S3" s="26">
+        <f>S40/AI35</f>
+        <v>0.99999031445728681</v>
+      </c>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="140"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA3" s="26">
+        <f>AA40/AI35</f>
+        <v>1.9999806289145736</v>
+      </c>
+      <c r="AB3" s="27"/>
+      <c r="AC3" s="27"/>
+      <c r="AD3" s="28"/>
+      <c r="AE3" s="140"/>
+      <c r="AF3" s="27"/>
+      <c r="AH3" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI3" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ3" s="67" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:36" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B4" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="141"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="56"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="141"/>
+      <c r="P4" s="123"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="S4" s="56"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="141"/>
+      <c r="X4" s="123"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA4" s="56"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="54"/>
+      <c r="AE4" s="141"/>
+      <c r="AF4" s="123"/>
+      <c r="AH4" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI4" s="15">
+        <v>115.03</v>
+      </c>
+      <c r="AJ4" s="16">
+        <v>115.03</v>
+      </c>
+    </row>
+    <row r="5" spans="2:36" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="141"/>
+      <c r="H5" s="123" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="141"/>
+      <c r="P5" s="123" t="s">
+        <v>128</v>
+      </c>
+      <c r="R5" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="S5" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="U5" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="W5" s="141"/>
+      <c r="X5" s="123" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z5" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB5" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC5" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD5" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE5" s="141"/>
+      <c r="AF5" s="123" t="s">
+        <v>128</v>
+      </c>
+      <c r="AH5" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI5" s="15">
+        <v>101.11</v>
+      </c>
+      <c r="AJ5" s="16">
+        <f>AI5*2</f>
+        <v>202.22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:36" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B6" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="51">
+        <v>1</v>
+      </c>
+      <c r="D6" s="51">
+        <v>115.3</v>
+      </c>
+      <c r="E6" s="51">
+        <v>0</v>
+      </c>
+      <c r="F6" s="53">
+        <f t="shared" ref="F6:F8" si="0">IF(OR(D6=0,E6=0),0,(D6*1000)/(1000/(C6*E6)))</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="142" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6">
+        <f>E6*20</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" s="51">
+        <v>1</v>
+      </c>
+      <c r="L6" s="51">
+        <v>115.3</v>
+      </c>
+      <c r="M6" s="51">
+        <v>0.5</v>
+      </c>
+      <c r="N6" s="53">
+        <f t="shared" ref="N6:N8" si="1">IF(OR(L6=0,M6=0),0,(L6*1000)/(1000/(K6*M6)))</f>
+        <v>57.65</v>
+      </c>
+      <c r="O6" s="142" t="s">
+        <v>129</v>
+      </c>
+      <c r="P6">
+        <f>M6*20</f>
+        <v>10</v>
+      </c>
+      <c r="R6" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="S6" s="51">
+        <v>1</v>
+      </c>
+      <c r="T6" s="51">
+        <v>115.3</v>
+      </c>
+      <c r="U6" s="51">
+        <v>1</v>
+      </c>
+      <c r="V6" s="53">
+        <f t="shared" ref="V6:V8" si="2">IF(OR(T6=0,U6=0),0,(T6*1000)/(1000/(S6*U6)))</f>
+        <v>115.3</v>
+      </c>
+      <c r="W6" s="142" t="s">
+        <v>129</v>
+      </c>
+      <c r="X6">
+        <f>U6*20</f>
+        <v>20</v>
+      </c>
+      <c r="Z6" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA6" s="51">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="51">
+        <v>115.3</v>
+      </c>
+      <c r="AC6" s="51">
+        <v>2</v>
+      </c>
+      <c r="AD6" s="53">
+        <f t="shared" ref="AD6:AD8" si="3">IF(OR(AB6=0,AC6=0),0,(AB6*1000)/(1000/(AA6*AC6)))</f>
+        <v>230.6</v>
+      </c>
+      <c r="AE6" s="142" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF6">
+        <f>AC6*20</f>
+        <v>40</v>
+      </c>
+      <c r="AH6" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI6" s="15">
+        <v>236.15</v>
+      </c>
+      <c r="AJ6" s="16">
+        <f>AI6*2</f>
+        <v>472.3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:36" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B7" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="22">
+        <v>2</v>
+      </c>
+      <c r="D7" s="22">
+        <v>101.1</v>
+      </c>
+      <c r="E7" s="22">
+        <v>2</v>
+      </c>
+      <c r="F7" s="30">
+        <f t="shared" si="0"/>
+        <v>404.4</v>
+      </c>
+      <c r="G7" s="142" t="s">
+        <v>130</v>
+      </c>
+      <c r="H7">
+        <f>E7*20</f>
+        <v>40</v>
+      </c>
+      <c r="J7" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="K7" s="22">
+        <v>2</v>
+      </c>
+      <c r="L7" s="22">
+        <v>101.1</v>
+      </c>
+      <c r="M7" s="22">
+        <v>2</v>
+      </c>
+      <c r="N7" s="30">
+        <f t="shared" si="1"/>
+        <v>404.4</v>
+      </c>
+      <c r="O7" s="142" t="s">
+        <v>130</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ref="P7:P9" si="4">M7*20</f>
+        <v>40</v>
+      </c>
+      <c r="R7" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="S7" s="22">
+        <v>2</v>
+      </c>
+      <c r="T7" s="22">
+        <v>101.1</v>
+      </c>
+      <c r="U7" s="22">
+        <v>2</v>
+      </c>
+      <c r="V7" s="30">
+        <f t="shared" si="2"/>
+        <v>404.4</v>
+      </c>
+      <c r="W7" s="142" t="s">
+        <v>130</v>
+      </c>
+      <c r="X7">
+        <f t="shared" ref="X7:X9" si="5">U7*20</f>
+        <v>40</v>
+      </c>
+      <c r="Z7" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA7" s="22">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="22">
+        <v>101.1</v>
+      </c>
+      <c r="AC7" s="22">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="30">
+        <f t="shared" si="3"/>
+        <v>404.4</v>
+      </c>
+      <c r="AE7" s="142" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF7">
+        <f t="shared" ref="AF7:AF9" si="6">AC7*20</f>
+        <v>40</v>
+      </c>
+      <c r="AH7" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI7" s="15">
+        <v>80.040000000000006</v>
+      </c>
+      <c r="AJ7" s="16">
+        <v>80.040000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="2:36" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B8" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="110">
+        <v>2</v>
+      </c>
+      <c r="D8" s="22">
+        <v>164.08799999999999</v>
+      </c>
+      <c r="E8" s="22">
+        <v>2</v>
+      </c>
+      <c r="F8" s="30">
+        <f t="shared" si="0"/>
+        <v>656.35199999999998</v>
+      </c>
+      <c r="G8" s="142" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8">
+        <f>E8*20</f>
+        <v>40</v>
+      </c>
+      <c r="J8" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="K8" s="22">
+        <v>2</v>
+      </c>
+      <c r="L8" s="22">
+        <v>164.08799999999999</v>
+      </c>
+      <c r="M8" s="22">
+        <v>1.75</v>
+      </c>
+      <c r="N8" s="30">
+        <f t="shared" si="1"/>
+        <v>574.30799999999999</v>
+      </c>
+      <c r="O8" s="142" t="s">
+        <v>131</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="R8" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="S8" s="22">
+        <v>2</v>
+      </c>
+      <c r="T8" s="22">
+        <v>164.08799999999999</v>
+      </c>
+      <c r="U8" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="V8" s="30">
+        <f t="shared" si="2"/>
+        <v>492.26400000000001</v>
+      </c>
+      <c r="W8" s="142" t="s">
+        <v>131</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="Z8" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA8" s="22">
+        <v>2</v>
+      </c>
+      <c r="AB8" s="22">
+        <v>164.08799999999999</v>
+      </c>
+      <c r="AC8" s="22">
+        <v>1.6</v>
+      </c>
+      <c r="AD8" s="30">
+        <f t="shared" si="3"/>
+        <v>525.08159999999998</v>
+      </c>
+      <c r="AE8" s="142" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="AH8" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI8" s="15">
+        <v>80.040000000000006</v>
+      </c>
+      <c r="AJ8" s="16">
+        <f>AI8*8</f>
+        <v>640.32000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="2:36" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B9" s="109" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="22">
+        <v>1</v>
+      </c>
+      <c r="D9" s="112">
+        <v>80.043000000000006</v>
+      </c>
+      <c r="E9" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="30">
+        <f>IF(OR(D9=0,E9=0),0,(D9*1000)/(1000/(C9*E9)))</f>
+        <v>120.06450000000001</v>
+      </c>
+      <c r="G9" s="146" t="s">
+        <v>132</v>
+      </c>
+      <c r="H9">
+        <f>E9*20</f>
+        <v>30</v>
+      </c>
+      <c r="J9" s="109" t="s">
+        <v>101</v>
+      </c>
+      <c r="K9" s="22">
+        <v>1</v>
+      </c>
+      <c r="L9" s="22">
+        <v>80.043000000000006</v>
+      </c>
+      <c r="M9" s="22">
+        <v>1.75</v>
+      </c>
+      <c r="N9" s="30">
+        <f>IF(OR(L9=0,M9=0),0,(L9*1000)/(1000/(K9*M9)))</f>
+        <v>140.07524999999998</v>
+      </c>
+      <c r="O9" s="146" t="s">
+        <v>132</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="R9" s="109" t="s">
+        <v>101</v>
+      </c>
+      <c r="S9" s="22">
+        <v>1</v>
+      </c>
+      <c r="T9" s="22">
+        <v>80.043000000000006</v>
+      </c>
+      <c r="U9" s="22">
+        <v>2</v>
+      </c>
+      <c r="V9" s="30">
+        <f>IF(OR(T9=0,U9=0),0,(T9*1000)/(1000/(S9*U9)))</f>
+        <v>160.08600000000001</v>
+      </c>
+      <c r="W9" s="142" t="s">
+        <v>132</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="Z9" s="109" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA9" s="22">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="22">
+        <v>80.043000000000006</v>
+      </c>
+      <c r="AC9" s="22">
+        <v>1.3</v>
+      </c>
+      <c r="AD9" s="30">
+        <f>IF(OR(AB9=0,AC9=0),0,(AB9*1000)/(1000/(AA9*AC9)))</f>
+        <v>104.05590000000001</v>
+      </c>
+      <c r="AE9" s="142" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF9">
+        <f t="shared" si="6"/>
+        <v>26</v>
+      </c>
+      <c r="AH9" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI9" s="15">
+        <v>136.09</v>
+      </c>
+      <c r="AJ9" s="16">
+        <v>136.09</v>
+      </c>
+    </row>
+    <row r="10" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="142"/>
+      <c r="J10" s="31"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="142"/>
+      <c r="R10" s="31"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="142"/>
+      <c r="Z10" s="31"/>
+      <c r="AD10" s="32"/>
+      <c r="AE10" s="142"/>
+      <c r="AH10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI10" s="15">
+        <v>74.55</v>
+      </c>
+      <c r="AJ10" s="16">
+        <v>74.55</v>
+      </c>
+    </row>
+    <row r="11" spans="2:36" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B11" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="141"/>
+      <c r="J11" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="141"/>
+      <c r="R11" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="S11" s="43"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="54"/>
+      <c r="W11" s="141"/>
+      <c r="X11" s="123"/>
+      <c r="Z11" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA11" s="43"/>
+      <c r="AB11" s="43"/>
+      <c r="AC11" s="43"/>
+      <c r="AD11" s="54"/>
+      <c r="AE11" s="141"/>
+      <c r="AF11" s="123"/>
+      <c r="AH11" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI11" s="15">
+        <v>100.09</v>
+      </c>
+      <c r="AJ11" s="16">
+        <v>100.09</v>
+      </c>
+    </row>
+    <row r="12" spans="2:36" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="141"/>
+      <c r="H12" s="123" t="s">
+        <v>128</v>
+      </c>
+      <c r="J12" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" s="141"/>
+      <c r="P12" s="123" t="s">
+        <v>128</v>
+      </c>
+      <c r="R12" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="S12" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="U12" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="V12" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="W12" s="141"/>
+      <c r="X12" s="123" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z12" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB12" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC12" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD12" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE12" s="141"/>
+      <c r="AF12" s="123" t="s">
+        <v>128</v>
+      </c>
+      <c r="AH12" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI12" s="15">
+        <v>246.48</v>
+      </c>
+      <c r="AJ12" s="16">
+        <f>AI12*2</f>
+        <v>492.96</v>
+      </c>
+    </row>
+    <row r="13" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="92" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="51">
+        <v>1</v>
+      </c>
+      <c r="D13" s="51">
+        <v>136.08600000000001</v>
+      </c>
+      <c r="E13" s="51">
+        <v>0</v>
+      </c>
+      <c r="F13" s="52">
+        <f>IF(OR(C13=0, E13=0), 0, (D13*1000)/(1000/(C13*E13)))</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="143" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13">
+        <f>E13*20</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="92" t="s">
+        <v>106</v>
+      </c>
+      <c r="K13" s="51">
+        <v>1</v>
+      </c>
+      <c r="L13" s="51">
+        <v>136.08600000000001</v>
+      </c>
+      <c r="M13" s="51">
+        <v>0</v>
+      </c>
+      <c r="N13" s="52">
+        <f>IF(OR(K13=0, M13=0), 0, (L13*1000)/(1000/(K13*M13)))</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="143" t="s">
+        <v>133</v>
+      </c>
+      <c r="P13">
+        <f>M13*20</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="92" t="s">
+        <v>106</v>
+      </c>
+      <c r="S13" s="51">
+        <v>1</v>
+      </c>
+      <c r="T13" s="51">
+        <v>136.08600000000001</v>
+      </c>
+      <c r="U13" s="51">
+        <v>0</v>
+      </c>
+      <c r="V13" s="52">
+        <v>0</v>
+      </c>
+      <c r="W13" s="143" t="s">
+        <v>133</v>
+      </c>
+      <c r="X13" s="35">
+        <f>U13*20</f>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="92" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA13" s="51">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="51">
+        <v>136.08600000000001</v>
+      </c>
+      <c r="AC13" s="51">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="52">
+        <f>IF(OR(AA13=0, AC13=0), 0, (AB13*1000)/(1000/(AA13*AC13)))</f>
+        <v>0</v>
+      </c>
+      <c r="AE13" s="143" t="s">
+        <v>133</v>
+      </c>
+      <c r="AF13" s="35">
+        <f>AC13*20</f>
+        <v>0</v>
+      </c>
+      <c r="AH13" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI13" s="18">
+        <v>38.5</v>
+      </c>
+      <c r="AJ13" s="19">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:36" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="94" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="22">
+        <v>1</v>
+      </c>
+      <c r="D14" s="22">
+        <v>74.555000000000007</v>
+      </c>
+      <c r="E14" s="22">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <f t="shared" ref="F14:F16" si="7">IF(OR(C14=0, E14=0), 0, (D14*1000)/(1000/(C14*E14)))</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="143" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H18" si="8">E14*20</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="94" t="s">
+        <v>103</v>
+      </c>
+      <c r="K14" s="22">
+        <v>1</v>
+      </c>
+      <c r="L14" s="22">
+        <v>74.555000000000007</v>
+      </c>
+      <c r="M14" s="22">
+        <v>0</v>
+      </c>
+      <c r="N14" s="33">
+        <f t="shared" ref="N14:N16" si="9">IF(OR(K14=0, M14=0), 0, (L14*1000)/(1000/(K14*M14)))</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="143" t="s">
+        <v>134</v>
+      </c>
+      <c r="P14">
+        <f t="shared" ref="P14:P18" si="10">M14*20</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="94" t="s">
+        <v>103</v>
+      </c>
+      <c r="S14" s="22">
+        <v>1</v>
+      </c>
+      <c r="T14" s="22">
+        <v>74.555000000000007</v>
+      </c>
+      <c r="U14" s="22">
+        <v>0</v>
+      </c>
+      <c r="V14" s="33">
+        <v>0</v>
+      </c>
+      <c r="W14" s="143" t="s">
+        <v>134</v>
+      </c>
+      <c r="X14" s="35">
+        <f t="shared" ref="X14:X18" si="11">U14*20</f>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="94" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA14" s="22">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="22">
+        <v>74.555000000000007</v>
+      </c>
+      <c r="AC14" s="22">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="33">
+        <f t="shared" ref="AD14:AD16" si="12">IF(OR(AA14=0, AC14=0), 0, (AB14*1000)/(1000/(AA14*AC14)))</f>
+        <v>0</v>
+      </c>
+      <c r="AE14" s="143" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF14" s="35">
+        <f t="shared" ref="AF14:AF18" si="13">AC14*20</f>
+        <v>0</v>
+      </c>
+      <c r="AH14" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI14" s="68"/>
+      <c r="AJ14" s="69"/>
+    </row>
+    <row r="15" spans="2:36" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B15" s="95" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="22">
+        <v>1</v>
+      </c>
+      <c r="D15" s="22">
+        <v>100.087</v>
+      </c>
+      <c r="E15" s="22">
+        <v>0.04</v>
+      </c>
+      <c r="F15" s="33">
+        <f t="shared" si="7"/>
+        <v>4.0034799999999997</v>
+      </c>
+      <c r="G15" s="143" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
+      <c r="J15" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="K15" s="22">
+        <v>1</v>
+      </c>
+      <c r="L15" s="22">
+        <v>100.087</v>
+      </c>
+      <c r="M15" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="N15" s="33">
+        <f t="shared" si="9"/>
+        <v>50.043500000000002</v>
+      </c>
+      <c r="O15" s="143" t="s">
+        <v>135</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="R15" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="S15" s="22">
+        <v>1</v>
+      </c>
+      <c r="T15" s="22">
+        <v>100.087</v>
+      </c>
+      <c r="U15" s="22">
+        <v>1</v>
+      </c>
+      <c r="V15" s="33">
+        <v>0</v>
+      </c>
+      <c r="W15" s="143" t="s">
+        <v>135</v>
+      </c>
+      <c r="X15" s="35">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="Z15" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA15" s="22">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="22">
+        <v>100.087</v>
+      </c>
+      <c r="AC15" s="129">
+        <v>0.8</v>
+      </c>
+      <c r="AD15" s="33">
+        <f t="shared" si="12"/>
+        <v>80.069599999999994</v>
+      </c>
+      <c r="AE15" s="143" t="s">
+        <v>135</v>
+      </c>
+      <c r="AF15" s="35">
+        <f t="shared" si="13"/>
+        <v>16</v>
+      </c>
+      <c r="AH15" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI15" s="20">
+        <v>197.92</v>
+      </c>
+      <c r="AJ15" s="16">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:36" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B16" s="96" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="22">
+        <v>2</v>
+      </c>
+      <c r="D16" s="22">
+        <v>246.48</v>
+      </c>
+      <c r="E16" s="22">
+        <v>1</v>
+      </c>
+      <c r="F16" s="33">
+        <f t="shared" si="7"/>
+        <v>492.96</v>
+      </c>
+      <c r="G16" s="143" t="s">
+        <v>136</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="J16" s="96" t="s">
+        <v>108</v>
+      </c>
+      <c r="K16" s="22">
+        <v>2</v>
+      </c>
+      <c r="L16" s="22">
+        <v>246.48</v>
+      </c>
+      <c r="M16" s="22">
+        <v>1</v>
+      </c>
+      <c r="N16" s="33">
+        <f t="shared" si="9"/>
+        <v>492.96</v>
+      </c>
+      <c r="O16" s="143" t="s">
+        <v>136</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="R16" s="96" t="s">
+        <v>108</v>
+      </c>
+      <c r="S16" s="22">
+        <v>2</v>
+      </c>
+      <c r="T16" s="22">
+        <v>246.48</v>
+      </c>
+      <c r="U16" s="22">
+        <v>1</v>
+      </c>
+      <c r="V16" s="33">
+        <f t="shared" ref="V16:V18" si="14">(T16*1000)/(1000/(S16*U16))</f>
+        <v>492.96</v>
+      </c>
+      <c r="W16" s="143" t="s">
+        <v>136</v>
+      </c>
+      <c r="X16" s="35">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="Z16" s="96" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA16" s="22">
+        <v>2</v>
+      </c>
+      <c r="AB16" s="22">
+        <v>246.48</v>
+      </c>
+      <c r="AC16" s="22">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="33">
+        <f t="shared" si="12"/>
+        <v>492.96</v>
+      </c>
+      <c r="AE16" s="143" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF16" s="35">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="AH16" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI16" s="20">
+        <v>61.83</v>
+      </c>
+      <c r="AJ16" s="16">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="17" spans="2:36" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B17" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="22">
+        <v>1</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22">
+        <v>1</v>
+      </c>
+      <c r="F17" s="33"/>
+      <c r="G17" s="143" t="s">
+        <v>137</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="22">
+        <v>1</v>
+      </c>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22">
+        <v>1</v>
+      </c>
+      <c r="N17" s="33"/>
+      <c r="O17" s="143" t="s">
+        <v>137</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="R17" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="S17" s="22">
+        <v>1</v>
+      </c>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22">
+        <v>1</v>
+      </c>
+      <c r="V17" s="33">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="W17" s="143" t="s">
+        <v>137</v>
+      </c>
+      <c r="X17" s="35">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="Z17" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA17" s="22">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22">
+        <v>1</v>
+      </c>
+      <c r="AD17" s="33"/>
+      <c r="AE17" s="143" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF17" s="35">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="AH17" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI17" s="15">
+        <v>287.60000000000002</v>
+      </c>
+      <c r="AJ17" s="16">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:36" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="B18" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="22">
+        <v>1</v>
+      </c>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22">
+        <v>1</v>
+      </c>
+      <c r="F18" s="33">
+        <f t="shared" ref="F18" si="15">(D18*1000)/(1000/(C18*E18))</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="143" t="s">
+        <v>138</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" s="22">
+        <v>1</v>
+      </c>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22">
+        <v>1</v>
+      </c>
+      <c r="N18" s="33">
+        <f t="shared" ref="N18" si="16">(L18*1000)/(1000/(K18*M18))</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="143" t="s">
+        <v>138</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="R18" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="S18" s="22">
+        <v>1</v>
+      </c>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22">
+        <v>1</v>
+      </c>
+      <c r="V18" s="33">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="W18" s="143" t="s">
+        <v>138</v>
+      </c>
+      <c r="X18" s="35">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="Z18" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA18" s="22">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="22">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="33">
+        <f t="shared" ref="AD18" si="17">(AB18*1000)/(1000/(AA18*AC18))</f>
+        <v>0</v>
+      </c>
+      <c r="AE18" s="143" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF18" s="35">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="AH18" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI18" s="15">
+        <v>249.68</v>
+      </c>
+      <c r="AJ18" s="16">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="19" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="31"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="142"/>
+      <c r="J19" s="31"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="142"/>
+      <c r="R19" s="31"/>
+      <c r="V19" s="32"/>
+      <c r="W19" s="142"/>
+      <c r="Z19" s="31"/>
+      <c r="AD19" s="32"/>
+      <c r="AE19" s="142"/>
+      <c r="AH19" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI19" s="18">
+        <v>161.94999999999999</v>
+      </c>
+      <c r="AJ19" s="19">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="20" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="141"/>
+      <c r="H20" s="138"/>
+      <c r="J20" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="141"/>
+      <c r="P20" s="138"/>
+      <c r="R20" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="S20" s="43"/>
+      <c r="T20" s="43"/>
+      <c r="U20" s="43"/>
+      <c r="V20" s="54"/>
+      <c r="W20" s="141"/>
+      <c r="X20" s="138"/>
+      <c r="Z20" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA20" s="43"/>
+      <c r="AB20" s="43"/>
+      <c r="AC20" s="43"/>
+      <c r="AD20" s="54"/>
+      <c r="AE20" s="141"/>
+      <c r="AF20" s="138"/>
+      <c r="AH20" s="20"/>
+      <c r="AI20" s="15"/>
+      <c r="AJ20" s="20"/>
+    </row>
+    <row r="21" spans="2:36" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="141"/>
+      <c r="H21" s="138"/>
+      <c r="J21" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="M21" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="N21" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="141"/>
+      <c r="P21" s="138"/>
+      <c r="R21" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="S21" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="T21" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="U21" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="V21" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="W21" s="141"/>
+      <c r="X21" s="138"/>
+      <c r="Z21" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA21" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB21" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC21" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD21" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE21" s="141"/>
+      <c r="AF21" s="138"/>
+      <c r="AH21" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI21" s="75"/>
+      <c r="AJ21" s="76"/>
+    </row>
+    <row r="22" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="51">
+        <f>C6</f>
+        <v>1</v>
+      </c>
+      <c r="D22" s="51">
+        <v>14.006</v>
+      </c>
+      <c r="E22" s="51">
+        <f>E6</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="52">
+        <f t="shared" ref="F22:F35" si="18">IF(OR(C22=0, E22=0), 0, (D22*1000)/(1000/(C22*E22)))</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="143"/>
+      <c r="H22" s="35"/>
+      <c r="J22" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="K22" s="51">
+        <f>K6</f>
+        <v>1</v>
+      </c>
+      <c r="L22" s="51">
+        <v>14.006</v>
+      </c>
+      <c r="M22" s="51">
+        <f>M6</f>
+        <v>0.5</v>
+      </c>
+      <c r="N22" s="52">
+        <f>IF(OR(K22=0, M22=0), 0, (L22*1000)/(1000/(K22*M22)))</f>
+        <v>7.0030000000000001</v>
+      </c>
+      <c r="O22" s="143"/>
+      <c r="P22" s="35"/>
+      <c r="R22" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="S22" s="51">
+        <f>S6</f>
+        <v>1</v>
+      </c>
+      <c r="T22" s="51">
+        <v>14.006</v>
+      </c>
+      <c r="U22" s="51">
+        <f>U6</f>
+        <v>1</v>
+      </c>
+      <c r="V22" s="52">
+        <f>IF(OR(S22=0,U22=0),0,(T22*1000)/(1000/(S22*U22)))</f>
+        <v>14.006</v>
+      </c>
+      <c r="W22" s="143"/>
+      <c r="X22" s="35"/>
+      <c r="Z22" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA22" s="51">
+        <f>AA6</f>
+        <v>1</v>
+      </c>
+      <c r="AB22" s="51">
+        <v>14.006</v>
+      </c>
+      <c r="AC22" s="51">
+        <f>AC6</f>
+        <v>2</v>
+      </c>
+      <c r="AD22" s="52">
+        <f>IF(OR(AA22=0,AC22=0),0,(AB22*1000)/(1000/(AA22*AC22)))</f>
+        <v>28.012</v>
+      </c>
+      <c r="AE22" s="143"/>
+      <c r="AF22" s="35"/>
+      <c r="AH22" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI22" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ22" s="72" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B23" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="22">
+        <f>C6</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="22">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="E23" s="22">
+        <f>E6</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="33">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="143"/>
+      <c r="H23" s="35"/>
+      <c r="J23" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23" s="22">
+        <f>K6</f>
+        <v>1</v>
+      </c>
+      <c r="L23" s="22">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="M23" s="22">
+        <f>M6</f>
+        <v>0.5</v>
+      </c>
+      <c r="N23" s="33">
+        <f t="shared" ref="N23:N35" si="19">IF(OR(K23=0, M23=0), 0, (L23*1000)/(1000/(K23*M23)))</f>
+        <v>15.48685</v>
+      </c>
+      <c r="O23" s="143"/>
+      <c r="P23" s="35"/>
+      <c r="R23" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="S23" s="22">
+        <f>S6</f>
+        <v>1</v>
+      </c>
+      <c r="T23" s="22">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="U23" s="22">
+        <f>U6</f>
+        <v>1</v>
+      </c>
+      <c r="V23" s="33">
+        <f t="shared" ref="V23:V35" si="20">IF(OR(S23=0,U23=0),0,(T23*1000)/(1000/(S23*U23)))</f>
+        <v>30.973700000000001</v>
+      </c>
+      <c r="W23" s="143"/>
+      <c r="X23" s="35"/>
+      <c r="Z23" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA23" s="22">
+        <f>AA6</f>
+        <v>1</v>
+      </c>
+      <c r="AB23" s="22">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="AC23" s="22">
+        <f>AC6</f>
+        <v>2</v>
+      </c>
+      <c r="AD23" s="33">
+        <f t="shared" ref="AD23:AD35" si="21">IF(OR(AA23=0,AC23=0),0,(AB23*1000)/(1000/(AA23*AC23)))</f>
+        <v>61.947400000000002</v>
+      </c>
+      <c r="AE23" s="143"/>
+      <c r="AF23" s="35"/>
+      <c r="AH23" s="77" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI23" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ23" s="79"/>
+    </row>
+    <row r="24" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B24" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="22">
+        <f>C7</f>
+        <v>2</v>
+      </c>
+      <c r="D24" s="22">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="E24" s="22">
+        <f>E7</f>
+        <v>2</v>
+      </c>
+      <c r="F24" s="33">
+        <f t="shared" si="18"/>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="G24" s="143"/>
+      <c r="H24" s="35"/>
+      <c r="J24" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="K24" s="22">
+        <f>K7</f>
+        <v>2</v>
+      </c>
+      <c r="L24" s="22">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="M24" s="22">
+        <f>M7</f>
+        <v>2</v>
+      </c>
+      <c r="N24" s="33">
+        <f t="shared" si="19"/>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="O24" s="143"/>
+      <c r="P24" s="35"/>
+      <c r="R24" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="S24" s="22">
+        <f>S7</f>
+        <v>2</v>
+      </c>
+      <c r="T24" s="22">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="U24" s="22">
+        <f>U7</f>
+        <v>2</v>
+      </c>
+      <c r="V24" s="33">
+        <f t="shared" si="20"/>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="W24" s="143"/>
+      <c r="X24" s="35"/>
+      <c r="Z24" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA24" s="22">
+        <f>AA7</f>
+        <v>2</v>
+      </c>
+      <c r="AB24" s="22">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="AC24" s="22">
+        <f>AC7</f>
+        <v>2</v>
+      </c>
+      <c r="AD24" s="33">
+        <f t="shared" si="21"/>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="AE24" s="143"/>
+      <c r="AF24" s="35"/>
+      <c r="AH24" s="80" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI24" s="81" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ24" s="82" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B25" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="22">
+        <f>C7</f>
+        <v>2</v>
+      </c>
+      <c r="D25" s="22">
+        <v>14.006</v>
+      </c>
+      <c r="E25" s="22">
+        <f>E7</f>
+        <v>2</v>
+      </c>
+      <c r="F25" s="33">
+        <f t="shared" si="18"/>
+        <v>56.024000000000001</v>
+      </c>
+      <c r="G25" s="143"/>
+      <c r="H25" s="35"/>
+      <c r="J25" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="K25" s="22">
+        <f>K7</f>
+        <v>2</v>
+      </c>
+      <c r="L25" s="22">
+        <v>14.006</v>
+      </c>
+      <c r="M25" s="22">
+        <f>M7</f>
+        <v>2</v>
+      </c>
+      <c r="N25" s="33">
+        <f t="shared" si="19"/>
+        <v>56.024000000000001</v>
+      </c>
+      <c r="O25" s="143"/>
+      <c r="P25" s="35"/>
+      <c r="R25" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="S25" s="22">
+        <f>S7</f>
+        <v>2</v>
+      </c>
+      <c r="T25" s="22">
+        <v>14.006</v>
+      </c>
+      <c r="U25" s="22">
+        <f>U7</f>
+        <v>2</v>
+      </c>
+      <c r="V25" s="33">
+        <f t="shared" si="20"/>
+        <v>56.024000000000001</v>
+      </c>
+      <c r="W25" s="143"/>
+      <c r="X25" s="35"/>
+      <c r="Z25" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA25" s="22">
+        <f>AA7</f>
+        <v>2</v>
+      </c>
+      <c r="AB25" s="22">
+        <v>14.006</v>
+      </c>
+      <c r="AC25" s="22">
+        <f>AC7</f>
+        <v>2</v>
+      </c>
+      <c r="AD25" s="33">
+        <f t="shared" si="21"/>
+        <v>56.024000000000001</v>
+      </c>
+      <c r="AE25" s="143"/>
+      <c r="AF25" s="35"/>
+      <c r="AH25" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI25" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ25" s="85" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B26" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="22">
+        <f>C8</f>
+        <v>2</v>
+      </c>
+      <c r="D26" s="22">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="E26" s="22">
+        <f>E8</f>
+        <v>2</v>
+      </c>
+      <c r="F26" s="33">
+        <f t="shared" si="18"/>
+        <v>160.31200000000001</v>
+      </c>
+      <c r="G26" s="143"/>
+      <c r="H26" s="35"/>
+      <c r="J26" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="K26" s="22">
+        <f>K8</f>
+        <v>2</v>
+      </c>
+      <c r="L26" s="22">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="M26" s="22">
+        <f>M8</f>
+        <v>1.75</v>
+      </c>
+      <c r="N26" s="33">
+        <f t="shared" si="19"/>
+        <v>140.273</v>
+      </c>
+      <c r="O26" s="143"/>
+      <c r="P26" s="35"/>
+      <c r="R26" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="S26" s="22">
+        <f>S8</f>
+        <v>2</v>
+      </c>
+      <c r="T26" s="22">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="U26" s="22">
+        <f>U8</f>
+        <v>1.5</v>
+      </c>
+      <c r="V26" s="33">
+        <f t="shared" si="20"/>
+        <v>120.23400000000001</v>
+      </c>
+      <c r="W26" s="143"/>
+      <c r="X26" s="35"/>
+      <c r="Z26" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA26" s="22">
+        <f>AA8</f>
+        <v>2</v>
+      </c>
+      <c r="AB26" s="22">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="AC26" s="22">
+        <f>AC8</f>
+        <v>1.6</v>
+      </c>
+      <c r="AD26" s="33">
+        <f t="shared" si="21"/>
+        <v>128.24959999999999</v>
+      </c>
+      <c r="AE26" s="143"/>
+      <c r="AF26" s="35"/>
+      <c r="AH26" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI26" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ26" s="88" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B27" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="22">
+        <f>C8</f>
+        <v>2</v>
+      </c>
+      <c r="D27" s="22">
+        <v>28.012</v>
+      </c>
+      <c r="E27" s="22">
+        <f>E8</f>
+        <v>2</v>
+      </c>
+      <c r="F27" s="33">
+        <f t="shared" si="18"/>
+        <v>112.048</v>
+      </c>
+      <c r="G27" s="143"/>
+      <c r="H27" s="35"/>
+      <c r="J27" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="K27" s="22">
+        <f>K8</f>
+        <v>2</v>
+      </c>
+      <c r="L27" s="22">
+        <v>28.012</v>
+      </c>
+      <c r="M27" s="22">
+        <f>M8</f>
+        <v>1.75</v>
+      </c>
+      <c r="N27" s="33">
+        <f t="shared" si="19"/>
+        <v>98.042000000000002</v>
+      </c>
+      <c r="O27" s="143"/>
+      <c r="P27" s="35"/>
+      <c r="R27" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="S27" s="22">
+        <f>S8</f>
+        <v>2</v>
+      </c>
+      <c r="T27" s="22">
+        <v>28.012</v>
+      </c>
+      <c r="U27" s="22">
+        <f>U8</f>
+        <v>1.5</v>
+      </c>
+      <c r="V27" s="33">
+        <f t="shared" si="20"/>
+        <v>84.036000000000001</v>
+      </c>
+      <c r="W27" s="143"/>
+      <c r="X27" s="35"/>
+      <c r="Z27" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA27" s="22">
+        <f>AA8</f>
+        <v>2</v>
+      </c>
+      <c r="AB27" s="22">
+        <v>28.012</v>
+      </c>
+      <c r="AC27" s="22">
+        <f>AC8</f>
+        <v>1.6</v>
+      </c>
+      <c r="AD27" s="33">
+        <f t="shared" si="21"/>
+        <v>89.638400000000004</v>
+      </c>
+      <c r="AE27" s="143"/>
+      <c r="AF27" s="35"/>
+      <c r="AH27" s="21"/>
+      <c r="AI27" s="73"/>
+      <c r="AJ27" s="11"/>
+    </row>
+    <row r="28" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B28" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="22">
+        <f>C9</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="22">
+        <v>28.012</v>
+      </c>
+      <c r="E28" s="22">
+        <f>E9</f>
+        <v>1.5</v>
+      </c>
+      <c r="F28" s="33">
+        <f>IF(OR(C28=0, E28=0), 0, (D28*1000)/(1000/(C28*E28)))</f>
+        <v>42.018000000000001</v>
+      </c>
+      <c r="G28" s="143"/>
+      <c r="H28" s="35"/>
+      <c r="J28" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="K28" s="22">
+        <f>K9</f>
+        <v>1</v>
+      </c>
+      <c r="L28" s="22">
+        <v>28.012</v>
+      </c>
+      <c r="M28" s="22">
+        <f>M9</f>
+        <v>1.75</v>
+      </c>
+      <c r="N28" s="33">
+        <f t="shared" si="19"/>
+        <v>49.021000000000001</v>
+      </c>
+      <c r="O28" s="143"/>
+      <c r="P28" s="35"/>
+      <c r="R28" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="S28" s="22">
+        <f>S9</f>
+        <v>1</v>
+      </c>
+      <c r="T28" s="22">
+        <v>28.012</v>
+      </c>
+      <c r="U28" s="22">
+        <f>U9</f>
+        <v>2</v>
+      </c>
+      <c r="V28" s="33">
+        <f t="shared" si="20"/>
+        <v>56.024000000000001</v>
+      </c>
+      <c r="W28" s="143"/>
+      <c r="X28" s="35"/>
+      <c r="Z28" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA28" s="22">
+        <f>AA9</f>
+        <v>1</v>
+      </c>
+      <c r="AB28" s="22">
+        <v>28.012</v>
+      </c>
+      <c r="AC28" s="22">
+        <f>AC9</f>
+        <v>1.3</v>
+      </c>
+      <c r="AD28" s="33">
+        <f>IF(OR(AA28=0,AC28=0),0,(AB28*1000)/(1000/(AA28*AC28)))</f>
+        <v>36.415600000000005</v>
+      </c>
+      <c r="AE28" s="143"/>
+      <c r="AF28" s="35"/>
+      <c r="AH28" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI28" s="90" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ28" s="91" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B29" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="22">
+        <f>C13</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="22">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="E29" s="22">
+        <f>E13</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="33">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="143"/>
+      <c r="H29" s="35"/>
+      <c r="J29" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="K29" s="22">
+        <f>K13</f>
+        <v>1</v>
+      </c>
+      <c r="L29" s="22">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="M29" s="22">
+        <f>M13</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="33">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="143"/>
+      <c r="P29" s="35"/>
+      <c r="R29" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="S29" s="22">
+        <f>S13</f>
+        <v>1</v>
+      </c>
+      <c r="T29" s="22">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="U29" s="22">
+        <f>U13</f>
+        <v>0</v>
+      </c>
+      <c r="V29" s="33">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W29" s="143"/>
+      <c r="X29" s="35"/>
+      <c r="Z29" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA29" s="22">
+        <f>AA13</f>
+        <v>1</v>
+      </c>
+      <c r="AB29" s="22">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="AC29" s="22">
+        <f>AC13</f>
+        <v>0</v>
+      </c>
+      <c r="AD29" s="33">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE29" s="143"/>
+      <c r="AF29" s="35"/>
+      <c r="AH29" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI29" s="98" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ29" s="99" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B30" s="93" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="22">
+        <f>C13</f>
+        <v>1</v>
+      </c>
+      <c r="D30" s="22">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="E30" s="22">
+        <f>E13</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="33">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="143"/>
+      <c r="H30" s="35"/>
+      <c r="J30" s="93" t="s">
+        <v>84</v>
+      </c>
+      <c r="K30" s="22">
+        <f>K13</f>
+        <v>1</v>
+      </c>
+      <c r="L30" s="22">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="M30" s="22">
+        <f>M13</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="33">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="143"/>
+      <c r="P30" s="35"/>
+      <c r="R30" s="93" t="s">
+        <v>84</v>
+      </c>
+      <c r="S30" s="22">
+        <f>S13</f>
+        <v>1</v>
+      </c>
+      <c r="T30" s="22">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="U30" s="22">
+        <f>U13</f>
+        <v>0</v>
+      </c>
+      <c r="V30" s="33">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W30" s="143"/>
+      <c r="X30" s="35"/>
+      <c r="Z30" s="93" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA30" s="22">
+        <f>AA13</f>
+        <v>1</v>
+      </c>
+      <c r="AB30" s="22">
+        <v>30.973700000000001</v>
+      </c>
+      <c r="AC30" s="22">
+        <f>AC13</f>
+        <v>0</v>
+      </c>
+      <c r="AD30" s="33">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE30" s="143"/>
+      <c r="AF30" s="35"/>
+      <c r="AH30" s="100" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI30" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ30" s="102" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B31" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="22">
+        <f>C14</f>
+        <v>1</v>
+      </c>
+      <c r="D31" s="22">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="E31" s="22">
+        <f>E14</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="33">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="143"/>
+      <c r="H31" s="35"/>
+      <c r="J31" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="22">
+        <f>K14</f>
+        <v>1</v>
+      </c>
+      <c r="L31" s="22">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="M31" s="22">
+        <f>M14</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="33">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="143"/>
+      <c r="P31" s="35"/>
+      <c r="R31" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="S31" s="22">
+        <f>S14</f>
+        <v>1</v>
+      </c>
+      <c r="T31" s="22">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="U31" s="22">
+        <f>U14</f>
+        <v>0</v>
+      </c>
+      <c r="V31" s="33">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W31" s="143"/>
+      <c r="X31" s="35"/>
+      <c r="Z31" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA31" s="22">
+        <f>AA14</f>
+        <v>1</v>
+      </c>
+      <c r="AB31" s="22">
+        <v>39.094299999999997</v>
+      </c>
+      <c r="AC31" s="22">
+        <f>AC14</f>
+        <v>0</v>
+      </c>
+      <c r="AD31" s="33">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE31" s="143"/>
+      <c r="AF31" s="35"/>
+      <c r="AH31" s="103" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI31" s="104" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ31" s="105" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B32" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="22">
+        <f>C14</f>
+        <v>1</v>
+      </c>
+      <c r="D32" s="22">
+        <v>35.453000000000003</v>
+      </c>
+      <c r="E32" s="22">
+        <f>E14</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="33">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="143"/>
+      <c r="H32" s="35"/>
+      <c r="J32" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32" s="22">
+        <f>K14</f>
+        <v>1</v>
+      </c>
+      <c r="L32" s="22">
+        <v>35.453000000000003</v>
+      </c>
+      <c r="M32" s="22">
+        <f>M14</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="33">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O32" s="143"/>
+      <c r="P32" s="35"/>
+      <c r="R32" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="S32" s="22">
+        <f>S14</f>
+        <v>1</v>
+      </c>
+      <c r="T32" s="22">
+        <v>35.453000000000003</v>
+      </c>
+      <c r="U32" s="22">
+        <f>U14</f>
+        <v>0</v>
+      </c>
+      <c r="V32" s="33">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W32" s="143"/>
+      <c r="X32" s="35"/>
+      <c r="Z32" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA32" s="22">
+        <f>AA14</f>
+        <v>1</v>
+      </c>
+      <c r="AB32" s="22">
+        <v>35.453000000000003</v>
+      </c>
+      <c r="AC32" s="22">
+        <f>AC14</f>
+        <v>0</v>
+      </c>
+      <c r="AD32" s="33">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AE32" s="143"/>
+      <c r="AF32" s="35"/>
+      <c r="AH32" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI32" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ32" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B33" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="22">
+        <f>C15</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="22">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="E33" s="22">
+        <f>E15</f>
+        <v>0.04</v>
+      </c>
+      <c r="F33" s="33">
+        <f t="shared" si="18"/>
+        <v>1.6031200000000001</v>
+      </c>
+      <c r="G33" s="143"/>
+      <c r="H33" s="35"/>
+      <c r="J33" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="K33" s="22">
+        <f>K15</f>
+        <v>1</v>
+      </c>
+      <c r="L33" s="22">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="M33" s="22">
+        <f>M15</f>
+        <v>0.5</v>
+      </c>
+      <c r="N33" s="33">
+        <f t="shared" si="19"/>
+        <v>20.039000000000001</v>
+      </c>
+      <c r="O33" s="143"/>
+      <c r="P33" s="35"/>
+      <c r="R33" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="S33" s="22">
+        <f>S15</f>
+        <v>1</v>
+      </c>
+      <c r="T33" s="22">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="U33" s="22">
+        <f>U15</f>
+        <v>1</v>
+      </c>
+      <c r="V33" s="33">
+        <f t="shared" si="20"/>
+        <v>40.078000000000003</v>
+      </c>
+      <c r="W33" s="143"/>
+      <c r="X33" s="35"/>
+      <c r="Z33" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA33" s="22">
+        <f>AA15</f>
+        <v>1</v>
+      </c>
+      <c r="AB33" s="22">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="AC33" s="22">
+        <f>AC15</f>
+        <v>0.8</v>
+      </c>
+      <c r="AD33" s="33">
+        <f t="shared" si="21"/>
+        <v>32.062399999999997</v>
+      </c>
+      <c r="AE33" s="143"/>
+      <c r="AF33" s="35"/>
+      <c r="AH33" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI33" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ33" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B34" s="96" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="22">
+        <f>C16</f>
+        <v>2</v>
+      </c>
+      <c r="D34" s="22">
+        <v>24.305</v>
+      </c>
+      <c r="E34" s="22">
+        <f>E16</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="33">
+        <f t="shared" si="18"/>
+        <v>48.61</v>
+      </c>
+      <c r="G34" s="143"/>
+      <c r="H34" s="35"/>
+      <c r="J34" s="96" t="s">
+        <v>86</v>
+      </c>
+      <c r="K34" s="22">
+        <f>K16</f>
+        <v>2</v>
+      </c>
+      <c r="L34" s="22">
+        <v>24.305</v>
+      </c>
+      <c r="M34" s="22">
+        <f>M16</f>
+        <v>1</v>
+      </c>
+      <c r="N34" s="33">
+        <f t="shared" si="19"/>
+        <v>48.61</v>
+      </c>
+      <c r="O34" s="143"/>
+      <c r="P34" s="35"/>
+      <c r="R34" s="96" t="s">
+        <v>86</v>
+      </c>
+      <c r="S34" s="22">
+        <f>S16</f>
+        <v>2</v>
+      </c>
+      <c r="T34" s="22">
+        <v>24.305</v>
+      </c>
+      <c r="U34" s="22">
+        <f>U16</f>
+        <v>1</v>
+      </c>
+      <c r="V34" s="33">
+        <f t="shared" si="20"/>
+        <v>48.61</v>
+      </c>
+      <c r="W34" s="143"/>
+      <c r="X34" s="35"/>
+      <c r="Z34" s="96" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA34" s="22">
+        <f>AA16</f>
+        <v>2</v>
+      </c>
+      <c r="AB34" s="22">
+        <v>24.305</v>
+      </c>
+      <c r="AC34" s="22">
+        <f>AC16</f>
+        <v>1</v>
+      </c>
+      <c r="AD34" s="33">
+        <f t="shared" si="21"/>
+        <v>48.61</v>
+      </c>
+      <c r="AE34" s="143"/>
+      <c r="AF34" s="35"/>
+      <c r="AH34" s="21"/>
+      <c r="AI34" s="73"/>
+      <c r="AJ34" s="11"/>
+    </row>
+    <row r="35" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="96" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="22">
+        <f>C16</f>
+        <v>2</v>
+      </c>
+      <c r="D35" s="22">
+        <v>32.064999999999998</v>
+      </c>
+      <c r="E35" s="22">
+        <f>E16</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="33">
+        <f t="shared" si="18"/>
+        <v>64.13</v>
+      </c>
+      <c r="G35" s="143"/>
+      <c r="H35" s="35"/>
+      <c r="J35" s="96" t="s">
+        <v>87</v>
+      </c>
+      <c r="K35" s="22">
+        <f>K16</f>
+        <v>2</v>
+      </c>
+      <c r="L35" s="22">
+        <v>32.064999999999998</v>
+      </c>
+      <c r="M35" s="22">
+        <f>M16</f>
+        <v>1</v>
+      </c>
+      <c r="N35" s="33">
+        <f t="shared" si="19"/>
+        <v>64.13</v>
+      </c>
+      <c r="O35" s="143"/>
+      <c r="P35" s="35"/>
+      <c r="R35" s="96" t="s">
+        <v>87</v>
+      </c>
+      <c r="S35" s="22">
+        <f>S16</f>
+        <v>2</v>
+      </c>
+      <c r="T35" s="22">
+        <v>32.064999999999998</v>
+      </c>
+      <c r="U35" s="22">
+        <f>U16</f>
+        <v>1</v>
+      </c>
+      <c r="V35" s="33">
+        <f t="shared" si="20"/>
+        <v>64.13</v>
+      </c>
+      <c r="W35" s="143"/>
+      <c r="X35" s="35"/>
+      <c r="Z35" s="96" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA35" s="22">
+        <f>AA16</f>
+        <v>2</v>
+      </c>
+      <c r="AB35" s="22">
+        <v>32.064999999999998</v>
+      </c>
+      <c r="AC35" s="22">
+        <f>AC16</f>
+        <v>1</v>
+      </c>
+      <c r="AD35" s="33">
+        <f t="shared" si="21"/>
+        <v>64.13</v>
+      </c>
+      <c r="AE35" s="143"/>
+      <c r="AF35" s="35"/>
+      <c r="AH35" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI35" s="5">
+        <v>30.974</v>
+      </c>
+      <c r="AJ35" s="6"/>
+    </row>
+    <row r="36" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="31"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="143"/>
+      <c r="H36" s="35"/>
+      <c r="J36" s="31"/>
+      <c r="N36" s="34"/>
+      <c r="O36" s="143"/>
+      <c r="P36" s="35"/>
+      <c r="R36" s="31"/>
+      <c r="V36" s="34"/>
+      <c r="W36" s="143"/>
+      <c r="X36" s="35"/>
+      <c r="Z36" s="31"/>
+      <c r="AD36" s="34"/>
+      <c r="AE36" s="143"/>
+      <c r="AF36" s="35"/>
+    </row>
+    <row r="37" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B37" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="43"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="144"/>
+      <c r="H37" s="124"/>
+      <c r="J37" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="43"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="144"/>
+      <c r="P37" s="125"/>
+      <c r="R37" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="S37" s="43"/>
+      <c r="T37" s="44"/>
+      <c r="U37" s="44"/>
+      <c r="V37" s="50"/>
+      <c r="W37" s="147"/>
+      <c r="X37" s="125"/>
+      <c r="Z37" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA37" s="43"/>
+      <c r="AB37" s="44"/>
+      <c r="AC37" s="44"/>
+      <c r="AD37" s="50"/>
+      <c r="AE37" s="147"/>
+      <c r="AF37" s="125"/>
+    </row>
+    <row r="38" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="48"/>
+      <c r="E38" s="117" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" s="128" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" s="145"/>
+      <c r="H38" s="125"/>
+      <c r="J38" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="L38" s="48"/>
+      <c r="M38" s="117" t="s">
+        <v>95</v>
+      </c>
+      <c r="N38" s="128" t="s">
+        <v>97</v>
+      </c>
+      <c r="O38" s="145"/>
+      <c r="P38" s="125"/>
+      <c r="R38" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="S38" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="T38" s="48"/>
+      <c r="U38" s="117" t="s">
+        <v>95</v>
+      </c>
+      <c r="V38" s="128" t="s">
+        <v>97</v>
+      </c>
+      <c r="W38" s="145"/>
+      <c r="X38" s="125"/>
+      <c r="Z38" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA38" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB38" s="48"/>
+      <c r="AC38" s="117" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD38" s="128" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE38" s="145"/>
+      <c r="AF38" s="125"/>
+    </row>
+    <row r="39" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B39" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="120">
+        <f>SUM(F22,F25,F27,F28)</f>
+        <v>210.09</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="35">
+        <f>C48-C39</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="32">
+        <v>6.7</v>
+      </c>
+      <c r="G39" s="142"/>
+      <c r="J39" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" s="120">
+        <f>SUM(N22,N25,N27,N28)</f>
+        <v>210.09000000000003</v>
+      </c>
+      <c r="M39" s="35">
+        <f>C48-K39</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="32">
+        <v>6.79</v>
+      </c>
+      <c r="O39" s="142"/>
+      <c r="R39" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="S39" s="59">
+        <f>SUM(V22,V25,V27,V28)</f>
+        <v>210.09</v>
+      </c>
+      <c r="U39" s="118">
+        <f>S39-C48</f>
+        <v>0</v>
+      </c>
+      <c r="V39" s="32">
+        <v>6.7</v>
+      </c>
+      <c r="W39" s="142"/>
+      <c r="Z39" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA39" s="59">
+        <f>SUM(AD22,AD25,AD27,AD28)</f>
+        <v>210.09</v>
+      </c>
+      <c r="AC39" s="35">
+        <f>C48-AA39</f>
+        <v>0</v>
+      </c>
+      <c r="AD39" s="32">
+        <v>6.72</v>
+      </c>
+      <c r="AE39" s="142"/>
+    </row>
+    <row r="40" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B40" s="114" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="22">
+        <f>SUM(F23,F30)</f>
+        <v>0</v>
+      </c>
+      <c r="E40" s="35">
+        <f t="shared" ref="E40:E44" si="22">C49-C40</f>
+        <v>30.973700000000001</v>
+      </c>
+      <c r="F40" s="32"/>
+      <c r="G40" s="142"/>
+      <c r="J40" s="114" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="131">
+        <f>SUM(N23,N30)</f>
+        <v>15.48685</v>
+      </c>
+      <c r="M40" s="35">
+        <f>C49-K40</f>
+        <v>15.48685</v>
+      </c>
+      <c r="N40" s="32"/>
+      <c r="O40" s="142"/>
+      <c r="R40" s="114" t="s">
+        <v>16</v>
+      </c>
+      <c r="S40" s="22">
+        <f>SUM(V23,V30)</f>
+        <v>30.973700000000001</v>
+      </c>
+      <c r="U40" s="118">
+        <f>S40-C49</f>
+        <v>0</v>
+      </c>
+      <c r="V40" s="32"/>
+      <c r="W40" s="142"/>
+      <c r="Z40" s="114" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA40" s="22">
+        <f>SUM(AD23,AD30)</f>
+        <v>61.947400000000002</v>
+      </c>
+      <c r="AC40" s="35">
+        <f>C49-AA40</f>
+        <v>-30.973700000000001</v>
+      </c>
+      <c r="AD40" s="32"/>
+      <c r="AE40" s="142"/>
+    </row>
+    <row r="41" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B41" s="114" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="119">
+        <f>SUM(F24,F29,F31)</f>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="E41" s="35">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="32"/>
+      <c r="G41" s="142"/>
+      <c r="J41" s="114" t="s">
+        <v>17</v>
+      </c>
+      <c r="K41" s="57">
+        <f>SUM(N24,N29,N31)</f>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="M41" s="35">
+        <f>C50-K41</f>
+        <v>0</v>
+      </c>
+      <c r="N41" s="32"/>
+      <c r="O41" s="142"/>
+      <c r="R41" s="114" t="s">
+        <v>17</v>
+      </c>
+      <c r="S41" s="57">
+        <f>SUM(V24,V29,V31)</f>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="U41" s="118">
+        <f>S41-C50</f>
+        <v>0</v>
+      </c>
+      <c r="V41" s="32"/>
+      <c r="W41" s="142"/>
+      <c r="Z41" s="114" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA41" s="57">
+        <f>SUM(AD24,AD29,AD31)</f>
+        <v>156.37719999999999</v>
+      </c>
+      <c r="AC41" s="35">
+        <f>C50-AA41</f>
+        <v>0</v>
+      </c>
+      <c r="AD41" s="32"/>
+      <c r="AE41" s="142"/>
+    </row>
+    <row r="42" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B42" s="114" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="119">
+        <f>F26+F33</f>
+        <v>161.91512</v>
+      </c>
+      <c r="E42" s="35">
+        <f t="shared" si="22"/>
+        <v>-1.6031199999999899</v>
+      </c>
+      <c r="F42" s="32"/>
+      <c r="G42" s="142"/>
+      <c r="J42" s="114" t="s">
+        <v>18</v>
+      </c>
+      <c r="K42" s="57">
+        <f>N26+N33</f>
+        <v>160.31200000000001</v>
+      </c>
+      <c r="M42" s="35">
+        <f>C51-K42</f>
+        <v>0</v>
+      </c>
+      <c r="N42" s="32"/>
+      <c r="O42" s="142"/>
+      <c r="R42" s="114" t="s">
+        <v>18</v>
+      </c>
+      <c r="S42" s="57">
+        <f>V26+V33</f>
+        <v>160.31200000000001</v>
+      </c>
+      <c r="U42" s="118">
+        <f>S42-C51</f>
+        <v>0</v>
+      </c>
+      <c r="V42" s="32"/>
+      <c r="W42" s="142"/>
+      <c r="Z42" s="114" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA42" s="57">
+        <f>AD26+AD33</f>
+        <v>160.31199999999998</v>
+      </c>
+      <c r="AC42" s="35">
+        <f>C51-AA42</f>
+        <v>0</v>
+      </c>
+      <c r="AD42" s="32"/>
+      <c r="AE42" s="142"/>
+    </row>
+    <row r="43" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B43" s="114" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="57">
+        <f>F34</f>
+        <v>48.61</v>
+      </c>
+      <c r="E43" s="35">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="32"/>
+      <c r="G43" s="142"/>
+      <c r="J43" s="114" t="s">
+        <v>19</v>
+      </c>
+      <c r="K43" s="57">
+        <f>N34</f>
+        <v>48.61</v>
+      </c>
+      <c r="M43" s="35">
+        <f>C52-K43</f>
+        <v>0</v>
+      </c>
+      <c r="N43" s="32"/>
+      <c r="O43" s="142"/>
+      <c r="R43" s="114" t="s">
+        <v>19</v>
+      </c>
+      <c r="S43" s="57">
+        <f>V34</f>
+        <v>48.61</v>
+      </c>
+      <c r="U43" s="118">
+        <f>S43-C52</f>
+        <v>0</v>
+      </c>
+      <c r="V43" s="32"/>
+      <c r="W43" s="142"/>
+      <c r="Z43" s="114" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA43" s="57">
+        <f>AD34</f>
+        <v>48.61</v>
+      </c>
+      <c r="AC43" s="35">
+        <f>C52-AA43</f>
+        <v>0</v>
+      </c>
+      <c r="AD43" s="32"/>
+      <c r="AE43" s="142"/>
+    </row>
+    <row r="44" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="115" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="58">
+        <f>F35</f>
+        <v>64.13</v>
+      </c>
+      <c r="D44" s="36"/>
+      <c r="E44" s="35">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="38"/>
+      <c r="G44" s="142"/>
+      <c r="J44" s="115" t="s">
+        <v>20</v>
+      </c>
+      <c r="K44" s="58">
+        <f>N35</f>
+        <v>64.13</v>
+      </c>
+      <c r="L44" s="36"/>
+      <c r="M44" s="35">
+        <f>C53-K44</f>
+        <v>0</v>
+      </c>
+      <c r="N44" s="38"/>
+      <c r="O44" s="142"/>
+      <c r="R44" s="115" t="s">
+        <v>20</v>
+      </c>
+      <c r="S44" s="58">
+        <f>V35</f>
+        <v>64.13</v>
+      </c>
+      <c r="T44" s="36"/>
+      <c r="U44" s="118">
+        <f>S44-C53</f>
+        <v>0</v>
+      </c>
+      <c r="V44" s="38"/>
+      <c r="W44" s="142"/>
+      <c r="Z44" s="115" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA44" s="58">
+        <f>AD35</f>
+        <v>64.13</v>
+      </c>
+      <c r="AB44" s="36"/>
+      <c r="AC44" s="35">
+        <f>C53-AA44</f>
+        <v>0</v>
+      </c>
+      <c r="AD44" s="38"/>
+      <c r="AE44" s="142"/>
+    </row>
+    <row r="47" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B47" s="116" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48">
+        <v>210.09</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49">
+        <v>30.973700000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50">
+        <v>156.37719999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51">
+        <v>160.31200000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52">
+        <v>48.61</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53">
+        <v>64.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E39:E44 M39:M44 U39:U44 AC39:AC44">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>-2</formula>
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="28" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B7E5A0-CE33-4932-A400-B881E6F8611C}">
   <dimension ref="B2:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-    <sheetView tabSelected="1" workbookViewId="2">
-      <selection activeCell="J27" sqref="J27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>